<commit_message>
add new testcase to TestLog
add new testcases for EditScreen (HomeScreen) of Remove-background module
</commit_message>
<xml_diff>
--- a/Log/Magic_eraser_test_log.xlsx
+++ b/Log/Magic_eraser_test_log.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18960" windowHeight="14740" activeTab="1"/>
+    <workbookView windowWidth="18960" windowHeight="14920" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Image_selector_test" sheetId="1" r:id="rId1"/>
@@ -3457,9 +3457,9 @@
   <dimension ref="A1:K84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.8"/>

</xml_diff>

<commit_message>
test RemoveBG homescreen update
</commit_message>
<xml_diff>
--- a/Log/Magic_eraser_test_log.xlsx
+++ b/Log/Magic_eraser_test_log.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18960" windowHeight="14920" activeTab="1"/>
+    <workbookView windowWidth="19020" windowHeight="14880" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Image_selector_test" sheetId="1" r:id="rId1"/>
     <sheet name="Load_memory_output_test" sheetId="2" r:id="rId2"/>
+    <sheet name="Home_screen_Remove_background" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="331">
   <si>
     <t>TC</t>
   </si>
@@ -781,6 +782,246 @@
   </si>
   <si>
     <t>chuyển về màn hình "Saved", ảnh mới được lưu trong máy có độ dài cạnh lớn nhất là 3841, vẫn giữ nguyên tỷ lệ</t>
+  </si>
+  <si>
+    <t>Khả năng truy cập tính năng "Remove background"</t>
+  </si>
+  <si>
+    <t>Ở màn hình Home</t>
+  </si>
+  <si>
+    <t>Nhấn button "Remove Background"</t>
+  </si>
+  <si>
+    <t>Hiển thị bảng chọn ảnh (image selector)</t>
+  </si>
+  <si>
+    <t>Ở màn hình Home, phần giới thiệu chức năng (image carousel) đang hiển thị phông giới thiệu chức năng "Remove Backgound"(Xoá phông)</t>
+  </si>
+  <si>
+    <t>Nhấn vào phần "image carousel"</t>
+  </si>
+  <si>
+    <t>Bảng chọn ảnh ("Image Selector")</t>
+  </si>
+  <si>
+    <t>Ở bảng chọn ảnh (image selector)</t>
+  </si>
+  <si>
+    <t>Hệ thống hiện lên topic thông báo xử lý ("Processing")</t>
+  </si>
+  <si>
+    <t>các test case chi tiết của "image selector" đã được test ở các testcase nhóm chức năng "image selector" và chức năng "export size image"</t>
+  </si>
+  <si>
+    <t>Ở bảng chọn ảnh (image selector), người dùng đã cấp quyền cho App</t>
+  </si>
+  <si>
+    <t>Chọn button "Camera"</t>
+  </si>
+  <si>
+    <t>Hệ thống chuyển sang màn hình camera mặc định của IOS</t>
+  </si>
+  <si>
+    <t>Đã chụp ảnh từ IOS và chuyển về màn hình xác nhận chọn ảnh</t>
+  </si>
+  <si>
+    <t>Chọn button xác nhận</t>
+  </si>
+  <si>
+    <t>Trên màn hình có dialog thông báo đang xử lý ("Processing"), màn hình phía dưới được phủ lớp layer xám</t>
+  </si>
+  <si>
+    <t>Nhấn 1 nút bất kỳ ở màn hình dưới (đã được phủ xám)</t>
+  </si>
+  <si>
+    <t>Hệ thống không có phản hồi gì</t>
+  </si>
+  <si>
+    <t>Trên màn hình có dilog thông báo đang xử lý ("Processing"). thời gian xử lý &gt; 5 giây (fetch success)</t>
+  </si>
+  <si>
+    <t>Popup dialog thông báo lỗi "xử lý ảnh không thành công"</t>
+  </si>
+  <si>
+    <t>Đây là trường hợp rất khó xảy ra nhưng vẫn cần cân nhắc</t>
+  </si>
+  <si>
+    <t>Trên màn hình có dialog thông báo đang xử lý ("Processing"), máy bị ngắt kết nối internet giữu chừng (fetch fail)</t>
+  </si>
+  <si>
+    <t>Chuyển phase giữa màn hình "Home-Editor" và "Home"</t>
+  </si>
+  <si>
+    <t>Trên màn hình có dialog thông báo đang xử lý, API trả về kết quả xử lý (fetch thành công)</t>
+  </si>
+  <si>
+    <t>Chuyển về màn hình "Home-edit", kết quả tách nền hiển thị trên cutout và các template hiển thị tương ứng với kết quả trả về</t>
+  </si>
+  <si>
+    <t>Ở màn "Home-edit"</t>
+  </si>
+  <si>
+    <t>Chọn button "&lt;-"</t>
+  </si>
+  <si>
+    <t>Hiển thị dialog cảnh bảo đang thoát ra mà chưa lưu kết quả</t>
+  </si>
+  <si>
+    <t>Ở màn "Home-edit", trên màn đang có dialog cảnh báo thoát ra mà chưa lưu kết quả, màn hình bị 1 lớp layer xám phủ lên, các nút trên màn bị vô hiệu hoá</t>
+  </si>
+  <si>
+    <t>Chọn vùng bên ngoài 2 nút trên dialog</t>
+  </si>
+  <si>
+    <t>App không có phản hồi</t>
+  </si>
+  <si>
+    <t>Ở màn "Home-edit", trên màn đang có dialog cảnh báo thoát ra mà chưa lưu kết quả, màn hình bị 2 lớp layer xám phủ lên, các nút trên màn bị vô hiệu hoá</t>
+  </si>
+  <si>
+    <t>Chọn button tiếp tục chỉnh sửa</t>
+  </si>
+  <si>
+    <t>Ở lại màn "Home-edit", dialog cảnh báo biến mất</t>
+  </si>
+  <si>
+    <t>Ở màn "Home-edit", trên màn đang có dialog cảnh báo thoát ra mà chưa lưu kết quả, màn hình bị 3 lớp layer xám phủ lên, các nút trên màn bị vô hiệu hoá</t>
+  </si>
+  <si>
+    <t>chọn button xác nhận thoát ra</t>
+  </si>
+  <si>
+    <t>Trở về màn hình "Home"</t>
+  </si>
+  <si>
+    <t>Chuyển phase giữa 2 màn hình Home-editor và Edit-cutout</t>
+  </si>
+  <si>
+    <t>Ở màn "Home-editor"</t>
+  </si>
+  <si>
+    <t>Nhấn vào vùng "Cutout Edit"</t>
+  </si>
+  <si>
+    <t>Chuyển vào màn "Edit cutout", ở phần Hình ảnh các phần bị xoá được tô màu, có các nút chức năng tương ứng</t>
+  </si>
+  <si>
+    <t>Ở màn "Edit cutout", người dùng đã có các thao tác chỉnh sửa trước đó</t>
+  </si>
+  <si>
+    <t>Nhấn vào nút "&lt;-"</t>
+  </si>
+  <si>
+    <t>Hiển thị dialog cảnh báo chưa lưu kết quả chỉnh sửa</t>
+  </si>
+  <si>
+    <t>Ở màn "Edit cutout", người dùng chưa có bất kỳ thao tác chỉnh sửa trước đó</t>
+  </si>
+  <si>
+    <t>Trở về màn hình "Home - edit"</t>
+  </si>
+  <si>
+    <t>Ở màn "Edit cutout", trên màn hình đang hiện dialog cảnh báo chưa lưu kết quả chỉnh sửa</t>
+  </si>
+  <si>
+    <t>Nhấn vào vùng ngoài các button của dialog</t>
+  </si>
+  <si>
+    <t>Nhấn button tiếp tục chỉnh sửa</t>
+  </si>
+  <si>
+    <t>Ở lại màn "Edit-cutout", dialog cảnh báo biến mất</t>
+  </si>
+  <si>
+    <t>Nhấn button xác nhận thoát ra ngoài</t>
+  </si>
+  <si>
+    <t>Thoát ra ngoài màn hình "Home-editor", kết quả cutout không có thay đổi so với trước khi vào màn "Edit-cutout"</t>
+  </si>
+  <si>
+    <t>Nhấn button "Save"</t>
+  </si>
+  <si>
+    <t>Thoát ra ngoài màn hình "Home-editor", kết quả cutout được cập nhật dựa trên chỉnh sửa của người dùng</t>
+  </si>
+  <si>
+    <t>Test case chi tiết của chức năng xuất ảnh được viết ở testcase chức năng "export image size"</t>
+  </si>
+  <si>
+    <t>Ở màn "Home edit"</t>
+  </si>
+  <si>
+    <t>Nhấn vào chọn 1 option bất kỳ không thuộc nhóm option tuỳ chỉnh</t>
+  </si>
+  <si>
+    <t>vào màn hình "Editor" cơ bản, hình ảnh được căn chỉnh đúng vị trí của cutout so với ảnh gốc, kết quả trả về của option đúng với yêu cầu</t>
+  </si>
+  <si>
+    <t>chọn option Tuỳ chỉnh màu</t>
+  </si>
+  <si>
+    <t>Hiện ra bảng tuỳ chỉnh màu (gọi tắt là message tuỳ chỉnh màu)</t>
+  </si>
+  <si>
+    <t>Ở màn "Home edit", trên màn hình có message tuỳ chỉnh màu</t>
+  </si>
+  <si>
+    <t>nhấn vào vùng ngoài message tuỳ chỉnh màu</t>
+  </si>
+  <si>
+    <t>tùy chỉnh màu trên bảng tròn chọn màu</t>
+  </si>
+  <si>
+    <t>Tone màu trên 2 thanh điều chỉnh độ ‘trong suốt’ và ‘sắc độ’ cũng thay đổi trùng vs màu được chọn trên bảng chọn màu</t>
+  </si>
+  <si>
+    <t>thao tác với thanh điều chỉnh độ trong suốt</t>
+  </si>
+  <si>
+    <t>Thanh điều chỉnh độ trong suốt được cập nhật theo thao tác của người dùng</t>
+  </si>
+  <si>
+    <t>thao tác với thanh điều chỉnh sắc độ</t>
+  </si>
+  <si>
+    <t>Thanh điều chỉnh sắc độ được cập nhật theo thao tác của người dùng</t>
+  </si>
+  <si>
+    <t>nhấn button huỷ tuỳ chỉnh</t>
+  </si>
+  <si>
+    <t>message tuỳ chỉnh màu biến mất, trở về màn "Home edit"</t>
+  </si>
+  <si>
+    <t>nhấn button xác nhận tuỳ chỉnh</t>
+  </si>
+  <si>
+    <t>Chuyển vào màn hình "Edit" cơ bản, nền được chèn bằng phông màu đã tuỳ chỉnh</t>
+  </si>
+  <si>
+    <t>chọn option Tải ảnh lên</t>
+  </si>
+  <si>
+    <t>chuyển sang màn chọn ảnh</t>
+  </si>
+  <si>
+    <t>Ở màn chọn ảnh, chức năng đang sử dụng là"Remove background"</t>
+  </si>
+  <si>
+    <t>Chuyển vào màn hình "Edit" cơ bản, nền được thay bằng ảnh đã chọn, tỷ lệ ảnh được giữ nguyên so với lần chọn size gần nhất</t>
+  </si>
+  <si>
+    <t>chọn option thuộc nhóm group (có nhiều lựa chọn đơn trong nhóm)</t>
+  </si>
+  <si>
+    <t>Hiện lên bảng chọn ảnh có các ảnh thuộc nhóm</t>
+  </si>
+  <si>
+    <t>tương tự như bảng "image selector" nhưng chỉ có các ảnh mà app cung cấp sẵn</t>
+  </si>
+  <si>
+    <t>Ở màn "Home edit", trên màn đang có bảng chọn ảnh</t>
   </si>
 </sst>
 </file>
@@ -1181,6 +1422,19 @@
       <left style="thin">
         <color auto="1"/>
       </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right/>
       <top style="thin">
         <color auto="1"/>
@@ -1199,19 +1453,6 @@
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -1544,10 +1785,43 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1563,13 +1837,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1581,10 +1855,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2144,1299 +2415,1299 @@
   <dimension ref="A1:L61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="F52" sqref="F52:F61"/>
+      <selection pane="bottomLeft" activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.8"/>
   <cols>
-    <col min="1" max="1" width="4" style="2" customWidth="1"/>
-    <col min="2" max="2" width="31.2890625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" style="3" customWidth="1"/>
-    <col min="4" max="5" width="24.4296875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="30.2890625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="20.140625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="4"/>
-    <col min="9" max="9" width="17.7109375" style="4" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="4" style="13" customWidth="1"/>
+    <col min="2" max="2" width="31.2890625" style="14" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" style="14" customWidth="1"/>
+    <col min="4" max="5" width="24.4296875" style="14" customWidth="1"/>
+    <col min="6" max="6" width="30.2890625" style="14" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" style="14" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="15"/>
+    <col min="9" max="9" width="17.7109375" style="15" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="15"/>
   </cols>
   <sheetData>
     <row r="1" ht="17.75" spans="1:7">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="29" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" ht="37" customHeight="1" spans="1:12">
-      <c r="A2" s="15">
+      <c r="A2" s="25">
         <v>1</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="18" t="s">
+      <c r="D2" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="18"/>
-      <c r="I2" s="20" t="s">
+      <c r="G2" s="28"/>
+      <c r="I2" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="20" t="s">
+      <c r="K2" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="20"/>
+      <c r="L2" s="30"/>
     </row>
     <row r="3" ht="34" spans="1:12">
-      <c r="A3" s="2">
+      <c r="A3" s="13">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="D3" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="20"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20"/>
+      <c r="I3" s="30"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="30"/>
     </row>
     <row r="4" ht="34" spans="1:12">
-      <c r="A4" s="2">
+      <c r="A4" s="13">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      <c r="D4" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="20"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="20"/>
+      <c r="I4" s="30"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="30"/>
     </row>
     <row r="5" ht="34" spans="1:12">
-      <c r="A5" s="2">
+      <c r="A5" s="13">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      <c r="D5" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="I5" s="20"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="20"/>
+      <c r="I5" s="30"/>
+      <c r="K5" s="30"/>
+      <c r="L5" s="30"/>
     </row>
     <row r="6" ht="34" spans="1:12">
-      <c r="A6" s="2">
+      <c r="A6" s="13">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="3" t="s">
+      <c r="D6" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="K6" s="20"/>
-      <c r="L6" s="20"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="30"/>
     </row>
     <row r="7" ht="17" spans="1:6">
-      <c r="A7" s="2">
+      <c r="A7" s="13">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="3" t="s">
+      <c r="D7" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="14" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="8" ht="50" customHeight="1" spans="1:6">
-      <c r="A8" s="2">
+      <c r="A8" s="13">
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="3" t="s">
+      <c r="D8" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="14" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" ht="34" spans="1:6">
-      <c r="A9" s="2">
+      <c r="A9" s="13">
         <v>8</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="3" t="s">
+      <c r="D9" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="14" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="10" ht="34" spans="1:6">
-      <c r="A10" s="2">
-        <v>9</v>
-      </c>
-      <c r="B10" s="3" t="s">
+      <c r="A10" s="13">
+        <v>9</v>
+      </c>
+      <c r="B10" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="3" t="s">
+      <c r="D10" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="14" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" ht="34" spans="1:6">
-      <c r="A11" s="2">
+      <c r="A11" s="13">
         <v>10</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="3" t="s">
+      <c r="D11" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="14" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="12" ht="34" spans="1:6">
-      <c r="A12" s="2">
+      <c r="A12" s="13">
         <v>11</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="3" t="s">
+      <c r="D12" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="14" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="13" ht="34" spans="1:6">
-      <c r="A13" s="2">
+      <c r="A13" s="13">
         <v>12</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="3" t="s">
+      <c r="D13" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="14" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="14" ht="51" spans="1:6">
-      <c r="A14" s="2">
+      <c r="A14" s="13">
         <v>13</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="3" t="s">
+      <c r="D14" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" s="14" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="15" ht="34" spans="1:6">
-      <c r="A15" s="2">
+      <c r="A15" s="13">
         <v>14</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" s="3" t="s">
+      <c r="D15" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F15" s="14" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="16" ht="34" spans="1:6">
-      <c r="A16" s="2">
+      <c r="A16" s="13">
         <v>15</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" s="3" t="s">
+      <c r="D16" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F16" s="14" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="17" ht="34" spans="1:6">
-      <c r="A17" s="2">
+      <c r="A17" s="13">
         <v>16</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" s="3" t="s">
+      <c r="D17" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F17" s="14" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="18" ht="34" spans="1:6">
-      <c r="A18" s="2">
+      <c r="A18" s="13">
         <v>17</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" s="3" t="s">
+      <c r="D18" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="F18" s="14" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="19" ht="34" spans="1:6">
-      <c r="A19" s="2">
+      <c r="A19" s="13">
         <v>18</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E19" s="3" t="s">
+      <c r="D19" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F19" s="14" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="20" ht="51" spans="1:6">
-      <c r="A20" s="2">
+      <c r="A20" s="13">
         <v>19</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E20" s="3" t="s">
+      <c r="D20" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F20" s="14" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="21" ht="34" spans="1:6">
-      <c r="A21" s="2">
+      <c r="A21" s="13">
         <v>20</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E21" s="3" t="s">
+      <c r="D21" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="F21" s="14" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="22" ht="34" spans="1:6">
-      <c r="A22" s="2">
+      <c r="A22" s="13">
         <v>21</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E22" s="3" t="s">
+      <c r="D22" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="F22" s="14" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="23" ht="34" spans="1:6">
-      <c r="A23" s="2">
+      <c r="A23" s="13">
         <v>22</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="D23" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E23" s="3" t="s">
+      <c r="D23" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F23" s="14" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="24" ht="34" spans="1:6">
-      <c r="A24" s="2">
+      <c r="A24" s="13">
         <v>23</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E24" s="3" t="s">
+      <c r="D24" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="F24" s="14" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="25" ht="34" spans="1:6">
-      <c r="A25" s="2">
+      <c r="A25" s="13">
         <v>24</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E25" s="3" t="s">
+      <c r="D25" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="F25" s="14" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="26" ht="34" spans="1:6">
-      <c r="A26" s="2">
+      <c r="A26" s="13">
         <v>25</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="D26" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E26" s="3" t="s">
+      <c r="D26" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="F26" s="14" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="27" ht="51" spans="1:6">
-      <c r="A27" s="2">
+      <c r="A27" s="13">
         <v>26</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="D27" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E27" s="3" t="s">
+      <c r="D27" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="F27" s="14" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="28" ht="51" spans="1:6">
-      <c r="A28" s="2">
+      <c r="A28" s="13">
         <v>27</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="D28" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E28" s="3" t="s">
+      <c r="D28" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="F28" s="14" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="29" ht="51" spans="1:6">
-      <c r="A29" s="2">
+      <c r="A29" s="13">
         <v>28</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="D29" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E29" s="3" t="s">
+      <c r="D29" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="F29" s="3" t="s">
+      <c r="F29" s="14" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="30" ht="51" spans="1:6">
-      <c r="A30" s="2">
+      <c r="A30" s="13">
         <v>29</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="D30" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E30" s="3" t="s">
+      <c r="D30" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="F30" s="3" t="s">
+      <c r="F30" s="14" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="31" ht="51" spans="1:6">
-      <c r="A31" s="2">
+      <c r="A31" s="13">
         <v>30</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D31" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="E31" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="F31" s="3" t="s">
+      <c r="F31" s="14" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="32" ht="51" spans="1:6">
-      <c r="A32" s="2">
+      <c r="A32" s="13">
         <v>31</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D32" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="E32" s="3" t="s">
+      <c r="E32" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="F32" s="3" t="s">
+      <c r="F32" s="14" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="33" ht="51" spans="1:6">
-      <c r="A33" s="2">
+      <c r="A33" s="13">
         <v>32</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D33" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="E33" s="3" t="s">
+      <c r="E33" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="F33" s="3" t="s">
+      <c r="F33" s="14" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="34" ht="51" spans="1:6">
-      <c r="A34" s="2">
+      <c r="A34" s="13">
         <v>33</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D34" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="E34" s="3" t="s">
+      <c r="E34" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="F34" s="3" t="s">
+      <c r="F34" s="14" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="35" ht="34" spans="1:6">
-      <c r="A35" s="2">
+      <c r="A35" s="13">
         <v>34</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="D35" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E35" s="3" t="s">
+      <c r="D35" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="F35" s="3" t="s">
+      <c r="F35" s="14" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="36" ht="51" spans="1:7">
-      <c r="A36" s="2">
+      <c r="A36" s="13">
         <v>35</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C36" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="D36" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E36" s="3" t="s">
+      <c r="D36" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E36" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="F36" s="3" t="s">
+      <c r="F36" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="G36" s="2" t="s">
+      <c r="G36" s="13" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="37" ht="101" spans="1:7">
-      <c r="A37" s="2">
+      <c r="A37" s="13">
         <v>36</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C37" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="D37" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E37" s="3" t="s">
+      <c r="D37" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E37" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="F37" s="3" t="s">
+      <c r="F37" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="G37" s="2"/>
+      <c r="G37" s="13"/>
     </row>
     <row r="38" ht="101" spans="1:7">
-      <c r="A38" s="2">
+      <c r="A38" s="13">
         <v>37</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C38" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="D38" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E38" s="3" t="s">
+      <c r="D38" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E38" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="F38" s="3" t="s">
+      <c r="F38" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="G38" s="2"/>
+      <c r="G38" s="13"/>
     </row>
     <row r="39" ht="118" spans="1:7">
-      <c r="A39" s="2">
+      <c r="A39" s="13">
         <v>38</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C39" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="D39" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E39" s="3" t="s">
+      <c r="D39" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="F39" s="3" t="s">
+      <c r="F39" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="G39" s="2"/>
+      <c r="G39" s="13"/>
     </row>
     <row r="40" ht="51" spans="1:7">
-      <c r="A40" s="2">
+      <c r="A40" s="13">
         <v>39</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C40" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="D40" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E40" s="3" t="s">
+      <c r="D40" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E40" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="F40" s="3" t="s">
+      <c r="F40" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="G40" s="2"/>
+      <c r="G40" s="13"/>
     </row>
     <row r="41" ht="101" spans="1:7">
-      <c r="A41" s="2">
+      <c r="A41" s="13">
         <v>40</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B41" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C41" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="D41" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E41" s="3" t="s">
+      <c r="D41" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E41" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="F41" s="3" t="s">
+      <c r="F41" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="G41" s="3" t="s">
+      <c r="G41" s="14" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="42" ht="84" spans="1:7">
-      <c r="A42" s="2">
+      <c r="A42" s="13">
         <v>41</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B42" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C42" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="D42" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E42" s="3" t="s">
+      <c r="D42" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E42" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="F42" s="3" t="s">
+      <c r="F42" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="G42" s="3" t="s">
+      <c r="G42" s="14" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="43" ht="84" spans="1:7">
-      <c r="A43" s="2">
+      <c r="A43" s="13">
         <v>42</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B43" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C43" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="D43" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E43" s="3" t="s">
+      <c r="D43" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E43" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="F43" s="3" t="s">
+      <c r="F43" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="G43" s="3" t="s">
+      <c r="G43" s="14" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="44" ht="118" spans="1:7">
-      <c r="A44" s="2">
+      <c r="A44" s="13">
         <v>43</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B44" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C44" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="D44" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E44" s="3" t="s">
+      <c r="D44" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E44" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="F44" s="3" t="s">
+      <c r="F44" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="G44" s="3" t="s">
+      <c r="G44" s="14" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="45" ht="101" spans="1:7">
-      <c r="A45" s="2">
+      <c r="A45" s="13">
         <v>44</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B45" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C45" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="D45" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E45" s="3" t="s">
+      <c r="D45" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E45" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="F45" s="3" t="s">
+      <c r="F45" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="G45" s="3" t="s">
+      <c r="G45" s="14" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="46" ht="118" spans="1:7">
-      <c r="A46" s="2">
+      <c r="A46" s="13">
         <v>45</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B46" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="C46" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="D46" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E46" s="3" t="s">
+      <c r="D46" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E46" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="F46" s="3" t="s">
+      <c r="F46" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="G46" s="3" t="s">
+      <c r="G46" s="14" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="47" ht="118" spans="1:7">
-      <c r="A47" s="2">
+      <c r="A47" s="13">
         <v>46</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B47" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="C47" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="D47" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E47" s="3" t="s">
+      <c r="D47" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E47" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="F47" s="3" t="s">
+      <c r="F47" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="G47" s="3" t="s">
+      <c r="G47" s="14" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="48" ht="34" spans="1:7">
-      <c r="A48" s="2">
+      <c r="A48" s="13">
         <v>47</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B48" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="C48" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="D48" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E48" s="3" t="s">
+      <c r="D48" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E48" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="F48" s="3" t="s">
+      <c r="F48" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="G48" s="3" t="s">
+      <c r="G48" s="14" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="49" ht="34" spans="1:7">
-      <c r="A49" s="2">
+      <c r="A49" s="13">
         <v>48</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B49" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="C49" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="D49" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E49" s="3" t="s">
+      <c r="D49" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E49" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="F49" s="3" t="s">
+      <c r="F49" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="G49" s="3" t="s">
+      <c r="G49" s="14" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="50" ht="135" spans="1:7">
-      <c r="A50" s="2">
+      <c r="A50" s="13">
         <v>49</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B50" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="C50" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="D50" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E50" s="3" t="s">
+      <c r="D50" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E50" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="F50" s="3" t="s">
+      <c r="F50" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="G50" s="3" t="s">
+      <c r="G50" s="14" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="51" ht="34" spans="1:7">
-      <c r="A51" s="2">
+      <c r="A51" s="13">
         <v>50</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B51" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="C51" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="D51" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E51" s="3" t="s">
+      <c r="D51" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E51" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="F51" s="3" t="s">
+      <c r="F51" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="G51" s="3" t="s">
+      <c r="G51" s="14" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="52" ht="68" spans="1:7">
-      <c r="A52" s="2">
+      <c r="A52" s="13">
         <v>51</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="B52" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="C52" s="3" t="s">
+      <c r="C52" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="D52" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E52" s="3" t="s">
+      <c r="D52" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E52" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="F52" s="2" t="s">
+      <c r="F52" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="G52" s="2" t="s">
+      <c r="G52" s="13" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="53" ht="68" spans="1:7">
-      <c r="A53" s="2">
+      <c r="A53" s="13">
         <v>52</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="B53" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="C53" s="3" t="s">
+      <c r="C53" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="D53" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E53" s="3" t="s">
+      <c r="D53" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E53" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="F53" s="2"/>
-      <c r="G53" s="2"/>
+      <c r="F53" s="13"/>
+      <c r="G53" s="13"/>
     </row>
     <row r="54" ht="68" spans="1:7">
-      <c r="A54" s="2">
+      <c r="A54" s="13">
         <v>53</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="B54" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="C54" s="3" t="s">
+      <c r="C54" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="D54" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E54" s="3" t="s">
+      <c r="D54" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E54" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="F54" s="2"/>
-      <c r="G54" s="2"/>
+      <c r="F54" s="13"/>
+      <c r="G54" s="13"/>
     </row>
     <row r="55" ht="68" spans="1:7">
-      <c r="A55" s="2">
+      <c r="A55" s="13">
         <v>54</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B55" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="C55" s="3" t="s">
+      <c r="C55" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="D55" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E55" s="3" t="s">
+      <c r="D55" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E55" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="F55" s="2"/>
-      <c r="G55" s="2"/>
+      <c r="F55" s="13"/>
+      <c r="G55" s="13"/>
     </row>
     <row r="56" ht="68" spans="1:7">
-      <c r="A56" s="2">
+      <c r="A56" s="13">
         <v>55</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="B56" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="C56" s="3" t="s">
+      <c r="C56" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="D56" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E56" s="3" t="s">
+      <c r="D56" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E56" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="F56" s="2"/>
-      <c r="G56" s="2"/>
+      <c r="F56" s="13"/>
+      <c r="G56" s="13"/>
     </row>
     <row r="57" ht="68" spans="1:7">
-      <c r="A57" s="2">
+      <c r="A57" s="13">
         <v>56</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="B57" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="C57" s="3" t="s">
+      <c r="C57" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="D57" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E57" s="3" t="s">
+      <c r="D57" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E57" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="F57" s="2"/>
-      <c r="G57" s="2"/>
+      <c r="F57" s="13"/>
+      <c r="G57" s="13"/>
     </row>
     <row r="58" ht="68" spans="1:7">
-      <c r="A58" s="2">
+      <c r="A58" s="13">
         <v>57</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="B58" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="C58" s="3" t="s">
+      <c r="C58" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="D58" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E58" s="3" t="s">
+      <c r="D58" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E58" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="F58" s="2"/>
-      <c r="G58" s="2"/>
+      <c r="F58" s="13"/>
+      <c r="G58" s="13"/>
     </row>
     <row r="59" ht="68" spans="1:7">
-      <c r="A59" s="2">
+      <c r="A59" s="13">
         <v>58</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="B59" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="C59" s="3" t="s">
+      <c r="C59" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="D59" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E59" s="3" t="s">
+      <c r="D59" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E59" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="F59" s="2"/>
-      <c r="G59" s="2"/>
+      <c r="F59" s="13"/>
+      <c r="G59" s="13"/>
     </row>
     <row r="60" ht="68" spans="1:7">
-      <c r="A60" s="2">
+      <c r="A60" s="13">
         <v>59</v>
       </c>
-      <c r="B60" s="3" t="s">
+      <c r="B60" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="C60" s="3" t="s">
+      <c r="C60" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="D60" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E60" s="3" t="s">
+      <c r="D60" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E60" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="F60" s="2"/>
-      <c r="G60" s="2"/>
+      <c r="F60" s="13"/>
+      <c r="G60" s="13"/>
     </row>
     <row r="61" ht="68" spans="1:7">
-      <c r="A61" s="2">
+      <c r="A61" s="13">
         <v>60</v>
       </c>
-      <c r="B61" s="3" t="s">
+      <c r="B61" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="C61" s="3" t="s">
+      <c r="C61" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="D61" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E61" s="3" t="s">
+      <c r="D61" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E61" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="F61" s="2"/>
-      <c r="G61" s="2"/>
+      <c r="F61" s="13"/>
+      <c r="G61" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -3456,1574 +3727,1574 @@
   <sheetPr/>
   <dimension ref="A1:K84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="$A1:$XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.8"/>
   <cols>
-    <col min="1" max="1" width="5.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="34.140625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="26.859375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="24.859375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="26.140625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="26.2890625" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="5.140625" style="13" customWidth="1"/>
+    <col min="2" max="2" width="34.140625" style="14" customWidth="1"/>
+    <col min="3" max="3" width="26.859375" style="14" customWidth="1"/>
+    <col min="4" max="4" width="24.859375" style="14" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" style="14" customWidth="1"/>
+    <col min="6" max="6" width="26.2890625" style="14" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="15"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1" spans="1:6">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="16" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" s="1" customFormat="1" ht="20" customHeight="1" spans="1:6">
-      <c r="A2" s="6" t="s">
+    <row r="2" s="12" customFormat="1" ht="20" customHeight="1" spans="1:6">
+      <c r="A2" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="11"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="22"/>
     </row>
     <row r="3" ht="118" customHeight="1" spans="1:11">
-      <c r="A3" s="2">
+      <c r="A3" s="13">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="H3" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
     </row>
     <row r="4" ht="101" customHeight="1" spans="1:11">
-      <c r="A4" s="2">
+      <c r="A4" s="13">
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="E4" s="14"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
+      <c r="E4" s="24"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
     </row>
     <row r="5" ht="122" customHeight="1" spans="1:11">
-      <c r="A5" s="2">
+      <c r="A5" s="13">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="E5" s="14"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
+      <c r="E5" s="24"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
     </row>
     <row r="6" ht="84" spans="1:5">
-      <c r="A6" s="2">
+      <c r="A6" s="13">
         <v>4</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="E6" s="14"/>
+      <c r="E6" s="24"/>
     </row>
     <row r="7" customFormat="1" ht="84" spans="1:6">
-      <c r="A7" s="2">
+      <c r="A7" s="13">
         <v>5</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="E7" s="15"/>
-      <c r="F7" s="3"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="14"/>
     </row>
     <row r="8" customFormat="1" ht="84" spans="1:6">
-      <c r="A8" s="2">
+      <c r="A8" s="13">
         <v>6</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="23" t="s">
         <v>119</v>
       </c>
-      <c r="F8" s="3"/>
+      <c r="F8" s="14"/>
     </row>
     <row r="9" customFormat="1" ht="84" spans="1:6">
-      <c r="A9" s="2">
+      <c r="A9" s="13">
         <v>7</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="E9" s="14"/>
-      <c r="F9" s="3"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="14"/>
     </row>
     <row r="10" customFormat="1" ht="84" spans="1:6">
-      <c r="A10" s="2">
+      <c r="A10" s="13">
         <v>8</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="E10" s="14"/>
-      <c r="F10" s="3"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="14"/>
     </row>
     <row r="11" customFormat="1" ht="84" spans="1:6">
-      <c r="A11" s="2">
-        <v>9</v>
-      </c>
-      <c r="B11" s="3" t="s">
+      <c r="A11" s="13">
+        <v>9</v>
+      </c>
+      <c r="B11" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="E11" s="14"/>
-      <c r="F11" s="3"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="14"/>
     </row>
     <row r="12" customFormat="1" ht="84" spans="1:6">
-      <c r="A12" s="2">
+      <c r="A12" s="13">
         <v>10</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="E12" s="15"/>
-      <c r="F12" s="3"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="14"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
     </row>
     <row r="14" ht="84" spans="1:6">
-      <c r="A14" s="2">
+      <c r="A14" s="13">
         <v>11</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" s="14" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="15" ht="68" spans="1:6">
-      <c r="A15" s="2">
+      <c r="A15" s="13">
         <v>12</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E15" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F15" s="14" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="16" ht="68" spans="1:6">
-      <c r="A16" s="2">
+      <c r="A16" s="13">
         <v>13</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F16" s="14" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="17" ht="68" spans="1:6">
-      <c r="A17" s="2">
+      <c r="A17" s="13">
         <v>14</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F17" s="14" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="18" ht="90" customHeight="1" spans="1:6">
-      <c r="A18" s="2">
+      <c r="A18" s="13">
         <v>15</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="21" t="s">
         <v>137</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D18" s="21" t="s">
         <v>139</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E18" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="F18" s="10" t="s">
+      <c r="F18" s="21" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="19" ht="66" customHeight="1" spans="1:6">
-      <c r="A19" s="2">
+      <c r="A19" s="13">
         <v>16</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D19" s="21" t="s">
         <v>143</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E19" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="F19" s="10" t="s">
+      <c r="F19" s="21" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="20" ht="79" customHeight="1" spans="1:6">
-      <c r="A20" s="2">
+      <c r="A20" s="13">
         <v>17</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="21" t="s">
         <v>145</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="D20" s="21" t="s">
         <v>146</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E20" s="21" t="s">
         <v>147</v>
       </c>
-      <c r="F20" s="10" t="s">
+      <c r="F20" s="21" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="21" ht="80" customHeight="1" spans="1:6">
-      <c r="A21" s="2">
+      <c r="A21" s="13">
         <v>18</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C21" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="D21" s="10" t="s">
+      <c r="D21" s="21" t="s">
         <v>150</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="E21" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="F21" s="10" t="s">
+      <c r="F21" s="21" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="22" ht="17" customHeight="1" spans="1:6">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="20" t="s">
         <v>152</v>
       </c>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
+      <c r="B22" s="20"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
     </row>
     <row r="23" ht="84" spans="1:6">
-      <c r="A23" s="2">
+      <c r="A23" s="13">
         <v>19</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D23" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="E23" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F23" s="14" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="24" ht="68" spans="1:6">
-      <c r="A24" s="2">
+      <c r="A24" s="13">
         <v>20</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D24" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="E24" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="F24" s="14" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="25" ht="68" spans="1:6">
-      <c r="A25" s="2">
+      <c r="A25" s="13">
         <v>21</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D25" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="E25" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="F25" s="14" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="26" ht="68" spans="1:6">
-      <c r="A26" s="2">
+      <c r="A26" s="13">
         <v>22</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D26" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="E26" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="F26" s="14" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="27" ht="68" spans="1:6">
-      <c r="A27" s="2">
+      <c r="A27" s="13">
         <v>23</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="B27" s="21" t="s">
         <v>137</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C27" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="D27" s="10" t="s">
+      <c r="D27" s="21" t="s">
         <v>154</v>
       </c>
-      <c r="E27" s="10" t="s">
+      <c r="E27" s="21" t="s">
         <v>155</v>
       </c>
-      <c r="F27" s="10" t="s">
+      <c r="F27" s="21" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="28" ht="51" spans="1:6">
-      <c r="A28" s="2">
+      <c r="A28" s="13">
         <v>24</v>
       </c>
-      <c r="B28" s="10" t="s">
+      <c r="B28" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="C28" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="D28" s="10" t="s">
+      <c r="D28" s="21" t="s">
         <v>143</v>
       </c>
-      <c r="E28" s="10" t="s">
+      <c r="E28" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="F28" s="10" t="s">
+      <c r="F28" s="21" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="29" ht="68" spans="1:6">
-      <c r="A29" s="2">
+      <c r="A29" s="13">
         <v>25</v>
       </c>
-      <c r="B29" s="10" t="s">
+      <c r="B29" s="21" t="s">
         <v>145</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C29" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="D29" s="10" t="s">
+      <c r="D29" s="21" t="s">
         <v>146</v>
       </c>
-      <c r="E29" s="10" t="s">
+      <c r="E29" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="F29" s="10" t="s">
+      <c r="F29" s="21" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="30" ht="68" spans="1:6">
-      <c r="A30" s="2">
+      <c r="A30" s="13">
         <v>26</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="B30" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="C30" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="D30" s="10" t="s">
+      <c r="D30" s="21" t="s">
         <v>150</v>
       </c>
-      <c r="E30" s="10" t="s">
+      <c r="E30" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="F30" s="10" t="s">
+      <c r="F30" s="21" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="9" t="s">
+      <c r="A31" s="20" t="s">
         <v>159</v>
       </c>
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
     </row>
     <row r="32" ht="68" spans="1:6">
-      <c r="A32" s="2">
+      <c r="A32" s="13">
         <v>27</v>
       </c>
-      <c r="B32" s="10" t="s">
+      <c r="B32" s="21" t="s">
         <v>137</v>
       </c>
-      <c r="C32" s="10" t="s">
+      <c r="C32" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="D32" s="10" t="s">
+      <c r="D32" s="21" t="s">
         <v>154</v>
       </c>
-      <c r="E32" s="10" t="s">
+      <c r="E32" s="21" t="s">
         <v>160</v>
       </c>
-      <c r="F32" s="10" t="s">
+      <c r="F32" s="21" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="33" ht="51" spans="1:6">
-      <c r="A33" s="2">
+      <c r="A33" s="13">
         <v>28</v>
       </c>
-      <c r="B33" s="10" t="s">
+      <c r="B33" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="C33" s="10" t="s">
+      <c r="C33" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="D33" s="10" t="s">
+      <c r="D33" s="21" t="s">
         <v>143</v>
       </c>
-      <c r="E33" s="10" t="s">
+      <c r="E33" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="F33" s="10" t="s">
+      <c r="F33" s="21" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="34" ht="68" spans="1:6">
-      <c r="A34" s="2">
+      <c r="A34" s="13">
         <v>29</v>
       </c>
-      <c r="B34" s="10" t="s">
+      <c r="B34" s="21" t="s">
         <v>145</v>
       </c>
-      <c r="C34" s="10" t="s">
+      <c r="C34" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="D34" s="10" t="s">
+      <c r="D34" s="21" t="s">
         <v>161</v>
       </c>
-      <c r="E34" s="10" t="s">
+      <c r="E34" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="F34" s="10" t="s">
+      <c r="F34" s="21" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="35" ht="68" spans="1:6">
-      <c r="A35" s="2">
+      <c r="A35" s="13">
         <v>30</v>
       </c>
-      <c r="B35" s="10" t="s">
+      <c r="B35" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="C35" s="10" t="s">
+      <c r="C35" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="D35" s="10" t="s">
+      <c r="D35" s="21" t="s">
         <v>162</v>
       </c>
-      <c r="E35" s="10" t="s">
+      <c r="E35" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="F35" s="10" t="s">
+      <c r="F35" s="21" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="36" spans="1:6">
-      <c r="A36" s="9" t="s">
+      <c r="A36" s="20" t="s">
         <v>163</v>
       </c>
-      <c r="B36" s="9"/>
-      <c r="C36" s="9"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="9"/>
+      <c r="B36" s="20"/>
+      <c r="C36" s="20"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="20"/>
+      <c r="F36" s="20"/>
     </row>
     <row r="37" ht="84" spans="1:6">
-      <c r="A37" s="2">
+      <c r="A37" s="13">
         <v>31</v>
       </c>
-      <c r="B37" s="10" t="s">
+      <c r="B37" s="21" t="s">
         <v>137</v>
       </c>
-      <c r="C37" s="10" t="s">
+      <c r="C37" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="D37" s="10" t="s">
+      <c r="D37" s="21" t="s">
         <v>164</v>
       </c>
-      <c r="E37" s="10" t="s">
+      <c r="E37" s="21" t="s">
         <v>165</v>
       </c>
-      <c r="F37" s="10" t="s">
+      <c r="F37" s="21" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="38" ht="68" spans="1:6">
-      <c r="A38" s="2">
+      <c r="A38" s="13">
         <v>32</v>
       </c>
-      <c r="B38" s="10" t="s">
+      <c r="B38" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="C38" s="10" t="s">
+      <c r="C38" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="D38" s="10" t="s">
+      <c r="D38" s="21" t="s">
         <v>166</v>
       </c>
-      <c r="E38" s="10" t="s">
+      <c r="E38" s="21" t="s">
         <v>167</v>
       </c>
-      <c r="F38" s="10" t="s">
+      <c r="F38" s="21" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="39" ht="68" spans="1:6">
-      <c r="A39" s="2">
+      <c r="A39" s="13">
         <v>33</v>
       </c>
-      <c r="B39" s="10" t="s">
+      <c r="B39" s="21" t="s">
         <v>145</v>
       </c>
-      <c r="C39" s="10" t="s">
+      <c r="C39" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="D39" s="10" t="s">
+      <c r="D39" s="21" t="s">
         <v>168</v>
       </c>
-      <c r="E39" s="10" t="s">
+      <c r="E39" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="F39" s="10" t="s">
+      <c r="F39" s="21" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="40" ht="68" spans="1:6">
-      <c r="A40" s="2">
+      <c r="A40" s="13">
         <v>34</v>
       </c>
-      <c r="B40" s="10" t="s">
+      <c r="B40" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="C40" s="10" t="s">
+      <c r="C40" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="D40" s="10" t="s">
+      <c r="D40" s="21" t="s">
         <v>170</v>
       </c>
-      <c r="E40" s="10" t="s">
+      <c r="E40" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="F40" s="10" t="s">
+      <c r="F40" s="21" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="41" spans="1:6">
-      <c r="A41" s="9" t="s">
+      <c r="A41" s="20" t="s">
         <v>171</v>
       </c>
-      <c r="B41" s="9"/>
-      <c r="C41" s="9"/>
-      <c r="D41" s="9"/>
-      <c r="E41" s="9"/>
-      <c r="F41" s="9"/>
+      <c r="B41" s="20"/>
+      <c r="C41" s="20"/>
+      <c r="D41" s="20"/>
+      <c r="E41" s="20"/>
+      <c r="F41" s="20"/>
     </row>
     <row r="42" ht="84" spans="1:6">
-      <c r="A42" s="2">
+      <c r="A42" s="13">
         <v>35</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B42" s="14" t="s">
         <v>172</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C42" s="14" t="s">
         <v>173</v>
       </c>
-      <c r="D42" s="10" t="s">
+      <c r="D42" s="21" t="s">
         <v>174</v>
       </c>
-      <c r="E42" s="3" t="s">
+      <c r="E42" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="F42" s="3" t="s">
+      <c r="F42" s="14" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="43" ht="68" spans="1:6">
-      <c r="A43" s="2">
+      <c r="A43" s="13">
         <v>36</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B43" s="14" t="s">
         <v>176</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C43" s="14" t="s">
         <v>173</v>
       </c>
-      <c r="D43" s="10" t="s">
+      <c r="D43" s="21" t="s">
         <v>177</v>
       </c>
-      <c r="E43" s="3" t="s">
+      <c r="E43" s="14" t="s">
         <v>178</v>
       </c>
-      <c r="F43" s="3" t="s">
+      <c r="F43" s="14" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="44" ht="68" spans="1:6">
-      <c r="A44" s="2">
+      <c r="A44" s="13">
         <v>37</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B44" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C44" s="14" t="s">
         <v>173</v>
       </c>
-      <c r="D44" s="10" t="s">
+      <c r="D44" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="E44" s="3" t="s">
+      <c r="E44" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="F44" s="3" t="s">
+      <c r="F44" s="14" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="45" ht="68" spans="1:6">
-      <c r="A45" s="2">
+      <c r="A45" s="13">
         <v>38</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B45" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C45" s="14" t="s">
         <v>173</v>
       </c>
-      <c r="D45" s="10" t="s">
+      <c r="D45" s="21" t="s">
         <v>182</v>
       </c>
-      <c r="E45" s="3" t="s">
+      <c r="E45" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="F45" s="3" t="s">
+      <c r="F45" s="14" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="46" ht="68" spans="1:6">
-      <c r="A46" s="2">
+      <c r="A46" s="13">
         <v>39</v>
       </c>
-      <c r="B46" s="10" t="s">
+      <c r="B46" s="21" t="s">
         <v>137</v>
       </c>
-      <c r="C46" s="10" t="s">
+      <c r="C46" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="D46" s="10" t="s">
+      <c r="D46" s="21" t="s">
         <v>184</v>
       </c>
-      <c r="E46" s="10" t="s">
+      <c r="E46" s="21" t="s">
         <v>160</v>
       </c>
-      <c r="F46" s="10" t="s">
+      <c r="F46" s="21" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="47" ht="118" spans="1:6">
-      <c r="A47" s="2">
+      <c r="A47" s="13">
         <v>40</v>
       </c>
-      <c r="B47" s="10" t="s">
+      <c r="B47" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="C47" s="10" t="s">
+      <c r="C47" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="D47" s="10" t="s">
+      <c r="D47" s="21" t="s">
         <v>186</v>
       </c>
-      <c r="E47" s="10" t="s">
+      <c r="E47" s="21" t="s">
         <v>187</v>
       </c>
-      <c r="F47" s="10" t="s">
+      <c r="F47" s="21" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="48" ht="68" spans="1:6">
-      <c r="A48" s="2">
+      <c r="A48" s="13">
         <v>41</v>
       </c>
-      <c r="B48" s="10" t="s">
+      <c r="B48" s="21" t="s">
         <v>145</v>
       </c>
-      <c r="C48" s="10" t="s">
+      <c r="C48" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="D48" s="10" t="s">
+      <c r="D48" s="21" t="s">
         <v>189</v>
       </c>
-      <c r="E48" s="10" t="s">
+      <c r="E48" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="F48" s="10" t="s">
+      <c r="F48" s="21" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="49" ht="68" spans="1:6">
-      <c r="A49" s="2">
+      <c r="A49" s="13">
         <v>42</v>
       </c>
-      <c r="B49" s="10" t="s">
+      <c r="B49" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="C49" s="10" t="s">
+      <c r="C49" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="D49" s="10" t="s">
+      <c r="D49" s="21" t="s">
         <v>191</v>
       </c>
-      <c r="E49" s="10" t="s">
+      <c r="E49" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="F49" s="10" t="s">
+      <c r="F49" s="21" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="50" spans="1:6">
-      <c r="A50" s="9" t="s">
+      <c r="A50" s="20" t="s">
         <v>193</v>
       </c>
-      <c r="B50" s="9"/>
-      <c r="C50" s="9"/>
-      <c r="D50" s="9"/>
-      <c r="E50" s="9"/>
-      <c r="F50" s="9"/>
+      <c r="B50" s="20"/>
+      <c r="C50" s="20"/>
+      <c r="D50" s="20"/>
+      <c r="E50" s="20"/>
+      <c r="F50" s="20"/>
     </row>
     <row r="51" ht="68" spans="1:6">
-      <c r="A51" s="2">
+      <c r="A51" s="13">
         <v>43</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B51" s="14" t="s">
         <v>194</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="C51" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="D51" s="3" t="s">
+      <c r="D51" s="14" t="s">
         <v>195</v>
       </c>
-      <c r="E51" s="3" t="s">
+      <c r="E51" s="14" t="s">
         <v>196</v>
       </c>
-      <c r="F51" s="3" t="s">
+      <c r="F51" s="14" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="52" ht="68" spans="1:6">
-      <c r="A52" s="2">
+      <c r="A52" s="13">
         <v>44</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="B52" s="14" t="s">
         <v>198</v>
       </c>
-      <c r="C52" s="3" t="s">
+      <c r="C52" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="D52" s="3" t="s">
+      <c r="D52" s="14" t="s">
         <v>199</v>
       </c>
-      <c r="E52" s="3" t="s">
+      <c r="E52" s="14" t="s">
         <v>196</v>
       </c>
-      <c r="F52" s="3" t="s">
+      <c r="F52" s="14" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="53" ht="68" spans="1:6">
-      <c r="A53" s="2">
+      <c r="A53" s="13">
         <v>45</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="B53" s="14" t="s">
         <v>201</v>
       </c>
-      <c r="C53" s="3" t="s">
+      <c r="C53" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="D53" s="3" t="s">
+      <c r="D53" s="14" t="s">
         <v>202</v>
       </c>
-      <c r="E53" s="3" t="s">
+      <c r="E53" s="14" t="s">
         <v>196</v>
       </c>
-      <c r="F53" s="3" t="s">
+      <c r="F53" s="14" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="54" ht="68" spans="1:6">
-      <c r="A54" s="2">
+      <c r="A54" s="13">
         <v>46</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="B54" s="14" t="s">
         <v>204</v>
       </c>
-      <c r="C54" s="10" t="s">
+      <c r="C54" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="D54" s="10" t="s">
+      <c r="D54" s="21" t="s">
         <v>205</v>
       </c>
-      <c r="E54" s="10" t="s">
+      <c r="E54" s="21" t="s">
         <v>160</v>
       </c>
-      <c r="F54" s="10" t="s">
+      <c r="F54" s="21" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="55" ht="68" spans="1:6">
-      <c r="A55" s="2">
+      <c r="A55" s="13">
         <v>47</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B55" s="14" t="s">
         <v>206</v>
       </c>
-      <c r="C55" s="10" t="s">
+      <c r="C55" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="D55" s="10" t="s">
+      <c r="D55" s="21" t="s">
         <v>207</v>
       </c>
-      <c r="E55" s="10" t="s">
+      <c r="E55" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="F55" s="10" t="s">
+      <c r="F55" s="21" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="56" ht="68" spans="1:6">
-      <c r="A56" s="2">
+      <c r="A56" s="13">
         <v>48</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="B56" s="14" t="s">
         <v>208</v>
       </c>
-      <c r="C56" s="10" t="s">
+      <c r="C56" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="D56" s="10" t="s">
+      <c r="D56" s="21" t="s">
         <v>209</v>
       </c>
-      <c r="E56" s="10" t="s">
+      <c r="E56" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="F56" s="10" t="s">
+      <c r="F56" s="21" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="57" ht="68" spans="1:6">
-      <c r="A57" s="2">
+      <c r="A57" s="13">
         <v>49</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="B57" s="14" t="s">
         <v>210</v>
       </c>
-      <c r="C57" s="10" t="s">
+      <c r="C57" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="D57" s="10" t="s">
+      <c r="D57" s="21" t="s">
         <v>211</v>
       </c>
-      <c r="E57" s="10" t="s">
+      <c r="E57" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="F57" s="10" t="s">
+      <c r="F57" s="21" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="58" spans="1:6">
-      <c r="A58" s="9" t="s">
+      <c r="A58" s="20" t="s">
         <v>212</v>
       </c>
-      <c r="B58" s="9"/>
-      <c r="C58" s="9"/>
-      <c r="D58" s="9"/>
-      <c r="E58" s="9"/>
-      <c r="F58" s="9"/>
+      <c r="B58" s="20"/>
+      <c r="C58" s="20"/>
+      <c r="D58" s="20"/>
+      <c r="E58" s="20"/>
+      <c r="F58" s="20"/>
     </row>
     <row r="59" ht="84" spans="1:6">
-      <c r="A59" s="2">
+      <c r="A59" s="13">
         <v>50</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="B59" s="14" t="s">
         <v>172</v>
       </c>
-      <c r="C59" s="3" t="s">
+      <c r="C59" s="14" t="s">
         <v>173</v>
       </c>
-      <c r="D59" s="10" t="s">
+      <c r="D59" s="21" t="s">
         <v>213</v>
       </c>
-      <c r="E59" s="3" t="s">
+      <c r="E59" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="F59" s="3" t="s">
+      <c r="F59" s="14" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="60" ht="68" spans="1:6">
-      <c r="A60" s="2">
+      <c r="A60" s="13">
         <v>51</v>
       </c>
-      <c r="B60" s="3" t="s">
+      <c r="B60" s="14" t="s">
         <v>176</v>
       </c>
-      <c r="C60" s="3" t="s">
+      <c r="C60" s="14" t="s">
         <v>173</v>
       </c>
-      <c r="D60" s="10" t="s">
+      <c r="D60" s="21" t="s">
         <v>214</v>
       </c>
-      <c r="E60" s="3" t="s">
+      <c r="E60" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="F60" s="3" t="s">
+      <c r="F60" s="14" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="61" ht="68" spans="1:6">
-      <c r="A61" s="2">
+      <c r="A61" s="13">
         <v>52</v>
       </c>
-      <c r="B61" s="3" t="s">
+      <c r="B61" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="C61" s="3" t="s">
+      <c r="C61" s="14" t="s">
         <v>173</v>
       </c>
-      <c r="D61" s="10" t="s">
+      <c r="D61" s="21" t="s">
         <v>215</v>
       </c>
-      <c r="E61" s="3" t="s">
+      <c r="E61" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="F61" s="3" t="s">
+      <c r="F61" s="14" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="62" ht="68" spans="1:6">
-      <c r="A62" s="2">
+      <c r="A62" s="13">
         <v>53</v>
       </c>
-      <c r="B62" s="3" t="s">
+      <c r="B62" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="C62" s="3" t="s">
+      <c r="C62" s="14" t="s">
         <v>173</v>
       </c>
-      <c r="D62" s="10" t="s">
+      <c r="D62" s="21" t="s">
         <v>216</v>
       </c>
-      <c r="E62" s="3" t="s">
+      <c r="E62" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="F62" s="3" t="s">
+      <c r="F62" s="14" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="63" ht="68" spans="1:6">
-      <c r="A63" s="2">
+      <c r="A63" s="13">
         <v>54</v>
       </c>
-      <c r="B63" s="10" t="s">
+      <c r="B63" s="21" t="s">
         <v>137</v>
       </c>
-      <c r="C63" s="10" t="s">
+      <c r="C63" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="D63" s="10" t="s">
+      <c r="D63" s="21" t="s">
         <v>217</v>
       </c>
-      <c r="E63" s="10" t="s">
+      <c r="E63" s="21" t="s">
         <v>218</v>
       </c>
-      <c r="F63" s="10" t="s">
+      <c r="F63" s="21" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="64" ht="84" spans="1:6">
-      <c r="A64" s="2">
+      <c r="A64" s="13">
         <v>55</v>
       </c>
-      <c r="B64" s="10" t="s">
+      <c r="B64" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="C64" s="10" t="s">
+      <c r="C64" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="D64" s="10" t="s">
+      <c r="D64" s="21" t="s">
         <v>214</v>
       </c>
-      <c r="E64" s="10" t="s">
+      <c r="E64" s="21" t="s">
         <v>220</v>
       </c>
-      <c r="F64" s="10" t="s">
+      <c r="F64" s="21" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="65" ht="84" spans="1:6">
-      <c r="A65" s="2">
+      <c r="A65" s="13">
         <v>56</v>
       </c>
-      <c r="B65" s="10" t="s">
+      <c r="B65" s="21" t="s">
         <v>145</v>
       </c>
-      <c r="C65" s="10" t="s">
+      <c r="C65" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="D65" s="10" t="s">
+      <c r="D65" s="21" t="s">
         <v>221</v>
       </c>
-      <c r="E65" s="10" t="s">
+      <c r="E65" s="21" t="s">
         <v>220</v>
       </c>
-      <c r="F65" s="10" t="s">
+      <c r="F65" s="21" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="66" ht="68" spans="1:6">
-      <c r="A66" s="2">
+      <c r="A66" s="13">
         <v>57</v>
       </c>
-      <c r="B66" s="10" t="s">
+      <c r="B66" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="C66" s="10" t="s">
+      <c r="C66" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="D66" s="10" t="s">
+      <c r="D66" s="21" t="s">
         <v>222</v>
       </c>
-      <c r="E66" s="10" t="s">
+      <c r="E66" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="F66" s="10" t="s">
+      <c r="F66" s="21" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="67" spans="1:6">
-      <c r="A67" s="9" t="s">
+      <c r="A67" s="20" t="s">
         <v>223</v>
       </c>
-      <c r="B67" s="9"/>
-      <c r="C67" s="9"/>
-      <c r="D67" s="9"/>
-      <c r="E67" s="9"/>
-      <c r="F67" s="9"/>
+      <c r="B67" s="20"/>
+      <c r="C67" s="20"/>
+      <c r="D67" s="20"/>
+      <c r="E67" s="20"/>
+      <c r="F67" s="20"/>
     </row>
     <row r="68" ht="84" spans="1:6">
-      <c r="A68" s="2">
+      <c r="A68" s="13">
         <v>58</v>
       </c>
-      <c r="B68" s="3" t="s">
+      <c r="B68" s="14" t="s">
         <v>224</v>
       </c>
-      <c r="C68" s="3" t="s">
+      <c r="C68" s="14" t="s">
         <v>173</v>
       </c>
-      <c r="D68" s="10" t="s">
+      <c r="D68" s="21" t="s">
         <v>225</v>
       </c>
-      <c r="E68" s="3" t="s">
+      <c r="E68" s="14" t="s">
         <v>226</v>
       </c>
-      <c r="F68" s="3" t="s">
+      <c r="F68" s="14" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="69" ht="68" spans="1:6">
-      <c r="A69" s="2">
+      <c r="A69" s="13">
         <v>59</v>
       </c>
-      <c r="B69" s="3" t="s">
+      <c r="B69" s="14" t="s">
         <v>228</v>
       </c>
-      <c r="C69" s="3" t="s">
+      <c r="C69" s="14" t="s">
         <v>173</v>
       </c>
-      <c r="D69" s="10" t="s">
+      <c r="D69" s="21" t="s">
         <v>229</v>
       </c>
-      <c r="E69" s="3" t="s">
+      <c r="E69" s="14" t="s">
         <v>230</v>
       </c>
-      <c r="F69" s="3" t="s">
+      <c r="F69" s="14" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="70" ht="68" spans="1:6">
-      <c r="A70" s="2">
+      <c r="A70" s="13">
         <v>60</v>
       </c>
-      <c r="B70" s="3" t="s">
+      <c r="B70" s="14" t="s">
         <v>232</v>
       </c>
-      <c r="C70" s="3" t="s">
+      <c r="C70" s="14" t="s">
         <v>173</v>
       </c>
-      <c r="D70" s="10" t="s">
+      <c r="D70" s="21" t="s">
         <v>233</v>
       </c>
-      <c r="E70" s="3" t="s">
+      <c r="E70" s="14" t="s">
         <v>234</v>
       </c>
-      <c r="F70" s="3" t="s">
+      <c r="F70" s="14" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="71" ht="68" spans="1:6">
-      <c r="A71" s="2">
+      <c r="A71" s="13">
         <v>61</v>
       </c>
-      <c r="B71" s="3" t="s">
+      <c r="B71" s="14" t="s">
         <v>236</v>
       </c>
-      <c r="C71" s="3" t="s">
+      <c r="C71" s="14" t="s">
         <v>173</v>
       </c>
-      <c r="D71" s="10" t="s">
+      <c r="D71" s="21" t="s">
         <v>237</v>
       </c>
-      <c r="E71" s="3" t="s">
+      <c r="E71" s="14" t="s">
         <v>234</v>
       </c>
-      <c r="F71" s="3" t="s">
+      <c r="F71" s="14" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="72" ht="68" spans="1:6">
-      <c r="A72" s="2">
+      <c r="A72" s="13">
         <v>62</v>
       </c>
-      <c r="B72" s="10" t="s">
+      <c r="B72" s="21" t="s">
         <v>137</v>
       </c>
-      <c r="C72" s="10" t="s">
+      <c r="C72" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="D72" s="10" t="s">
+      <c r="D72" s="21" t="s">
         <v>239</v>
       </c>
-      <c r="E72" s="10" t="s">
+      <c r="E72" s="21" t="s">
         <v>240</v>
       </c>
-      <c r="F72" s="10" t="s">
+      <c r="F72" s="21" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="73" ht="68" spans="1:6">
-      <c r="A73" s="2">
+      <c r="A73" s="13">
         <v>63</v>
       </c>
-      <c r="B73" s="10" t="s">
+      <c r="B73" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="C73" s="10" t="s">
+      <c r="C73" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="D73" s="10" t="s">
+      <c r="D73" s="21" t="s">
         <v>229</v>
       </c>
-      <c r="E73" s="10" t="s">
+      <c r="E73" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="F73" s="10" t="s">
+      <c r="F73" s="21" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="74" ht="68" spans="1:6">
-      <c r="A74" s="2">
+      <c r="A74" s="13">
         <v>64</v>
       </c>
-      <c r="B74" s="10" t="s">
+      <c r="B74" s="21" t="s">
         <v>242</v>
       </c>
-      <c r="C74" s="10" t="s">
+      <c r="C74" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="D74" s="10" t="s">
+      <c r="D74" s="21" t="s">
         <v>243</v>
       </c>
-      <c r="E74" s="10" t="s">
+      <c r="E74" s="21" t="s">
         <v>244</v>
       </c>
-      <c r="F74" s="10" t="s">
+      <c r="F74" s="21" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="75" ht="68" spans="1:6">
-      <c r="A75" s="2">
+      <c r="A75" s="13">
         <v>65</v>
       </c>
-      <c r="B75" s="10" t="s">
+      <c r="B75" s="21" t="s">
         <v>245</v>
       </c>
-      <c r="C75" s="10" t="s">
+      <c r="C75" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="D75" s="10" t="s">
+      <c r="D75" s="21" t="s">
         <v>246</v>
       </c>
-      <c r="E75" s="10" t="s">
+      <c r="E75" s="21" t="s">
         <v>244</v>
       </c>
-      <c r="F75" s="10" t="s">
+      <c r="F75" s="21" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="76" spans="1:6">
-      <c r="A76" s="9" t="s">
+      <c r="A76" s="20" t="s">
         <v>247</v>
       </c>
-      <c r="B76" s="9"/>
-      <c r="C76" s="9"/>
-      <c r="D76" s="9"/>
-      <c r="E76" s="9"/>
-      <c r="F76" s="9"/>
+      <c r="B76" s="20"/>
+      <c r="C76" s="20"/>
+      <c r="D76" s="20"/>
+      <c r="E76" s="20"/>
+      <c r="F76" s="20"/>
     </row>
     <row r="77" ht="84" spans="1:6">
-      <c r="A77" s="2">
+      <c r="A77" s="13">
         <v>66</v>
       </c>
-      <c r="B77" s="3" t="s">
+      <c r="B77" s="14" t="s">
         <v>224</v>
       </c>
-      <c r="C77" s="3" t="s">
+      <c r="C77" s="14" t="s">
         <v>173</v>
       </c>
-      <c r="D77" s="10" t="s">
+      <c r="D77" s="21" t="s">
         <v>248</v>
       </c>
-      <c r="E77" s="3" t="s">
+      <c r="E77" s="14" t="s">
         <v>226</v>
       </c>
-      <c r="F77" s="3" t="s">
+      <c r="F77" s="14" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="78" ht="68" spans="1:6">
-      <c r="A78" s="2">
+      <c r="A78" s="13">
         <v>67</v>
       </c>
-      <c r="B78" s="3" t="s">
+      <c r="B78" s="14" t="s">
         <v>249</v>
       </c>
-      <c r="C78" s="3" t="s">
+      <c r="C78" s="14" t="s">
         <v>173</v>
       </c>
-      <c r="D78" s="10" t="s">
+      <c r="D78" s="21" t="s">
         <v>229</v>
       </c>
-      <c r="E78" s="3" t="s">
+      <c r="E78" s="14" t="s">
         <v>230</v>
       </c>
-      <c r="F78" s="3" t="s">
+      <c r="F78" s="14" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="79" ht="68" spans="1:6">
-      <c r="A79" s="2">
+      <c r="A79" s="13">
         <v>68</v>
       </c>
-      <c r="B79" s="3" t="s">
+      <c r="B79" s="14" t="s">
         <v>232</v>
       </c>
-      <c r="C79" s="3" t="s">
+      <c r="C79" s="14" t="s">
         <v>173</v>
       </c>
-      <c r="D79" s="10" t="s">
+      <c r="D79" s="21" t="s">
         <v>233</v>
       </c>
-      <c r="E79" s="3" t="s">
+      <c r="E79" s="14" t="s">
         <v>234</v>
       </c>
-      <c r="F79" s="3" t="s">
+      <c r="F79" s="14" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="80" ht="68" spans="1:6">
-      <c r="A80" s="2">
+      <c r="A80" s="13">
         <v>69</v>
       </c>
-      <c r="B80" s="3" t="s">
+      <c r="B80" s="14" t="s">
         <v>236</v>
       </c>
-      <c r="C80" s="3" t="s">
+      <c r="C80" s="14" t="s">
         <v>173</v>
       </c>
-      <c r="D80" s="10" t="s">
+      <c r="D80" s="21" t="s">
         <v>237</v>
       </c>
-      <c r="E80" s="3" t="s">
+      <c r="E80" s="14" t="s">
         <v>250</v>
       </c>
-      <c r="F80" s="3" t="s">
+      <c r="F80" s="14" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="81" ht="68" spans="1:6">
-      <c r="A81" s="2">
+      <c r="A81" s="13">
         <v>70</v>
       </c>
-      <c r="B81" s="10" t="s">
+      <c r="B81" s="21" t="s">
         <v>137</v>
       </c>
-      <c r="C81" s="10" t="s">
+      <c r="C81" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="D81" s="10" t="s">
+      <c r="D81" s="21" t="s">
         <v>239</v>
       </c>
-      <c r="E81" s="10" t="s">
+      <c r="E81" s="21" t="s">
         <v>160</v>
       </c>
-      <c r="F81" s="10" t="s">
+      <c r="F81" s="21" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="82" ht="68" spans="1:6">
-      <c r="A82" s="2">
+      <c r="A82" s="13">
         <v>71</v>
       </c>
-      <c r="B82" s="10" t="s">
+      <c r="B82" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="C82" s="10" t="s">
+      <c r="C82" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="D82" s="10" t="s">
+      <c r="D82" s="21" t="s">
         <v>229</v>
       </c>
-      <c r="E82" s="10" t="s">
+      <c r="E82" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="F82" s="10" t="s">
+      <c r="F82" s="21" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="83" ht="68" spans="1:6">
-      <c r="A83" s="2">
+      <c r="A83" s="13">
         <v>72</v>
       </c>
-      <c r="B83" s="10" t="s">
+      <c r="B83" s="21" t="s">
         <v>242</v>
       </c>
-      <c r="C83" s="10" t="s">
+      <c r="C83" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="D83" s="10" t="s">
+      <c r="D83" s="21" t="s">
         <v>243</v>
       </c>
-      <c r="E83" s="10" t="s">
+      <c r="E83" s="21" t="s">
         <v>244</v>
       </c>
-      <c r="F83" s="10" t="s">
+      <c r="F83" s="21" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="84" ht="68" spans="1:6">
-      <c r="A84" s="2">
+      <c r="A84" s="13">
         <v>73</v>
       </c>
-      <c r="B84" s="10" t="s">
+      <c r="B84" s="21" t="s">
         <v>245</v>
       </c>
-      <c r="C84" s="10" t="s">
+      <c r="C84" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="D84" s="10" t="s">
+      <c r="D84" s="21" t="s">
         <v>246</v>
       </c>
-      <c r="E84" s="10" t="s">
+      <c r="E84" s="21" t="s">
         <v>244</v>
       </c>
-      <c r="F84" s="10" t="s">
+      <c r="F84" s="21" t="s">
         <v>192</v>
       </c>
     </row>
@@ -5046,4 +5317,564 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="D44" sqref="D44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="5"/>
+  <cols>
+    <col min="1" max="1" width="4.296875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="26.953125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="23.1796875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="18.359375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="25.6484375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="18.875" style="4" customWidth="1"/>
+    <col min="7" max="16384" width="9" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" ht="20" customHeight="1" spans="1:6">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" s="2" customFormat="1" ht="20" customHeight="1" spans="1:6">
+      <c r="A2" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="11"/>
+    </row>
+    <row r="3" ht="34" spans="1:5">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="4" ht="84" spans="1:5">
+      <c r="A4" s="3">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="5" s="3" customFormat="1" spans="1:1">
+      <c r="A5" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="6" ht="34" spans="1:6">
+      <c r="A6" s="3">
+        <v>3</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="7" ht="51" spans="1:6">
+      <c r="A7" s="3">
+        <v>4</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="F7" s="9"/>
+    </row>
+    <row r="8" ht="51" spans="1:6">
+      <c r="A8" s="3">
+        <v>5</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="F8" s="9"/>
+    </row>
+    <row r="9" s="3" customFormat="1" spans="1:1">
+      <c r="A9" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" ht="68" spans="1:5">
+      <c r="A10" s="3">
+        <v>7</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="11" ht="68" spans="1:6">
+      <c r="A11" s="3">
+        <v>8</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="12" ht="68" spans="1:5">
+      <c r="A12" s="3">
+        <v>9</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="13" s="3" customFormat="1" spans="1:1">
+      <c r="A13" s="3" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="14" ht="84" spans="1:5">
+      <c r="A14" s="3">
+        <v>10</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="15" ht="34" spans="1:6">
+      <c r="A15" s="3">
+        <v>11</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="F15" s="9"/>
+    </row>
+    <row r="16" ht="84" spans="1:6">
+      <c r="A16" s="3">
+        <v>12</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>279</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9" t="s">
+        <v>281</v>
+      </c>
+      <c r="F16" s="9"/>
+    </row>
+    <row r="17" ht="84" spans="1:6">
+      <c r="A17" s="3">
+        <v>13</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>282</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>283</v>
+      </c>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9" t="s">
+        <v>284</v>
+      </c>
+      <c r="F17" s="9"/>
+    </row>
+    <row r="18" ht="84" spans="1:6">
+      <c r="A18" s="3">
+        <v>14</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>285</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="F18" s="9"/>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+    </row>
+    <row r="20" ht="85" customHeight="1" spans="1:5">
+      <c r="A20" s="3">
+        <v>15</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="21" ht="51" spans="1:5">
+      <c r="A21" s="3">
+        <v>16</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="22" ht="51" spans="1:5">
+      <c r="A22" s="3">
+        <v>17</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="23" ht="51" spans="1:5">
+      <c r="A23" s="3">
+        <v>18</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="24" ht="51" spans="1:5">
+      <c r="A24" s="3">
+        <v>19</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="25" ht="68" spans="1:5">
+      <c r="A25" s="3">
+        <v>20</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="26" ht="84" spans="1:6">
+      <c r="A26" s="3">
+        <v>21</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="27" ht="84" spans="1:5">
+      <c r="A27" s="3">
+        <v>22</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="28" ht="51" spans="1:5">
+      <c r="A28" s="3">
+        <v>23</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="29" ht="34" spans="1:5">
+      <c r="A29" s="3">
+        <v>24</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="30" ht="84" spans="1:5">
+      <c r="A30" s="3">
+        <v>25</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>313</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="31" ht="51" spans="1:5">
+      <c r="A31" s="3">
+        <v>26</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="32" ht="51" spans="1:5">
+      <c r="A32" s="3">
+        <v>27</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="33" ht="34" spans="1:5">
+      <c r="A33" s="3">
+        <v>28</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="34" ht="51" spans="1:5">
+      <c r="A34" s="3">
+        <v>29</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="35" ht="17" spans="1:5">
+      <c r="A35" s="3">
+        <v>30</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="36" ht="84" spans="1:5">
+      <c r="A36" s="3">
+        <v>31</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="37" ht="68" spans="1:6">
+      <c r="A37" s="3">
+        <v>32</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="38" ht="84" spans="1:5">
+      <c r="A38" s="3">
+        <v>33</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>326</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="A13:F13"/>
+    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="F6:F8"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix some wrong data
</commit_message>
<xml_diff>
--- a/Log/Magic_eraser_test_log.xlsx
+++ b/Log/Magic_eraser_test_log.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="332">
   <si>
     <t>TC</t>
   </si>
@@ -829,6 +829,9 @@
     <t>Chọn button xác nhận</t>
   </si>
   <si>
+    <t>Bước xử lý hình ảnh (fetch với server)</t>
+  </si>
+  <si>
     <t>Trên màn hình có dialog thông báo đang xử lý ("Processing"), màn hình phía dưới được phủ lớp layer xám</t>
   </si>
   <si>
@@ -847,7 +850,7 @@
     <t>Đây là trường hợp rất khó xảy ra nhưng vẫn cần cân nhắc</t>
   </si>
   <si>
-    <t>Trên màn hình có dialog thông báo đang xử lý ("Processing"), máy bị ngắt kết nối internet giữu chừng (fetch fail)</t>
+    <t>Trên màn hình có dialog thông báo đang xử lý ("Processing"), máy bị ngắt kết nối internet giữa chừng (fetch fail)</t>
   </si>
   <si>
     <t>Chuyển phase giữa màn hình "Home-Editor" và "Home"</t>
@@ -1785,7 +1788,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1796,9 +1799,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1813,9 +1813,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1831,9 +1828,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1875,9 +1869,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -2422,1292 +2413,1292 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.8"/>
   <cols>
-    <col min="1" max="1" width="4" style="13" customWidth="1"/>
-    <col min="2" max="2" width="31.2890625" style="14" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" style="14" customWidth="1"/>
-    <col min="4" max="5" width="24.4296875" style="14" customWidth="1"/>
-    <col min="6" max="6" width="30.2890625" style="14" customWidth="1"/>
-    <col min="7" max="7" width="20.140625" style="14" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="15"/>
-    <col min="9" max="9" width="17.7109375" style="15" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="15"/>
+    <col min="1" max="1" width="4" style="11" customWidth="1"/>
+    <col min="2" max="2" width="31.2890625" style="12" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" style="12" customWidth="1"/>
+    <col min="4" max="5" width="24.4296875" style="12" customWidth="1"/>
+    <col min="6" max="6" width="30.2890625" style="12" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" style="12" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="4"/>
+    <col min="9" max="9" width="17.7109375" style="4" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" ht="17.75" spans="1:7">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="G1" s="26" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" ht="37" customHeight="1" spans="1:12">
-      <c r="A2" s="25">
+      <c r="A2" s="22">
         <v>1</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="28" t="s">
+      <c r="D2" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="28" t="s">
+      <c r="F2" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="28"/>
-      <c r="I2" s="30" t="s">
+      <c r="G2" s="25"/>
+      <c r="I2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="30" t="s">
+      <c r="K2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="30"/>
+      <c r="L2" s="3"/>
     </row>
     <row r="3" ht="34" spans="1:12">
-      <c r="A3" s="13">
+      <c r="A3" s="11">
         <v>2</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="14" t="s">
+      <c r="D3" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="30"/>
-      <c r="K3" s="30"/>
-      <c r="L3" s="30"/>
+      <c r="I3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
     </row>
     <row r="4" ht="34" spans="1:12">
-      <c r="A4" s="13">
+      <c r="A4" s="11">
         <v>3</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="14" t="s">
+      <c r="D4" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="30"/>
-      <c r="K4" s="30"/>
-      <c r="L4" s="30"/>
+      <c r="I4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
     </row>
     <row r="5" ht="34" spans="1:12">
-      <c r="A5" s="13">
+      <c r="A5" s="11">
         <v>4</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="14" t="s">
+      <c r="D5" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="I5" s="30"/>
-      <c r="K5" s="30"/>
-      <c r="L5" s="30"/>
+      <c r="I5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
     </row>
     <row r="6" ht="34" spans="1:12">
-      <c r="A6" s="13">
+      <c r="A6" s="11">
         <v>5</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="14" t="s">
+      <c r="D6" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="K6" s="30"/>
-      <c r="L6" s="30"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
     </row>
     <row r="7" ht="17" spans="1:6">
-      <c r="A7" s="13">
+      <c r="A7" s="11">
         <v>6</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="14" t="s">
+      <c r="D7" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="12" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="8" ht="50" customHeight="1" spans="1:6">
-      <c r="A8" s="13">
+      <c r="A8" s="11">
         <v>7</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="14" t="s">
+      <c r="D8" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="12" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" ht="34" spans="1:6">
-      <c r="A9" s="13">
+      <c r="A9" s="11">
         <v>8</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="14" t="s">
+      <c r="D9" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="F9" s="12" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="10" ht="34" spans="1:6">
-      <c r="A10" s="13">
-        <v>9</v>
-      </c>
-      <c r="B10" s="14" t="s">
+      <c r="A10" s="11">
+        <v>9</v>
+      </c>
+      <c r="B10" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="14" t="s">
+      <c r="D10" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="14" t="s">
+      <c r="F10" s="12" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" ht="34" spans="1:6">
-      <c r="A11" s="13">
+      <c r="A11" s="11">
         <v>10</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="14" t="s">
+      <c r="D11" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="14" t="s">
+      <c r="F11" s="12" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="12" ht="34" spans="1:6">
-      <c r="A12" s="13">
+      <c r="A12" s="11">
         <v>11</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="14" t="s">
+      <c r="D12" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="14" t="s">
+      <c r="F12" s="12" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="13" ht="34" spans="1:6">
-      <c r="A13" s="13">
+      <c r="A13" s="11">
         <v>12</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="14" t="s">
+      <c r="D13" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="F13" s="14" t="s">
+      <c r="F13" s="12" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="14" ht="51" spans="1:6">
-      <c r="A14" s="13">
+      <c r="A14" s="11">
         <v>13</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="14" t="s">
+      <c r="D14" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="F14" s="14" t="s">
+      <c r="F14" s="12" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="15" ht="34" spans="1:6">
-      <c r="A15" s="13">
+      <c r="A15" s="11">
         <v>14</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" s="14" t="s">
+      <c r="D15" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="14" t="s">
+      <c r="F15" s="12" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="16" ht="34" spans="1:6">
-      <c r="A16" s="13">
+      <c r="A16" s="11">
         <v>15</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" s="14" t="s">
+      <c r="D16" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="F16" s="14" t="s">
+      <c r="F16" s="12" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="17" ht="34" spans="1:6">
-      <c r="A17" s="13">
+      <c r="A17" s="11">
         <v>16</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" s="14" t="s">
+      <c r="D17" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="F17" s="14" t="s">
+      <c r="F17" s="12" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="18" ht="34" spans="1:6">
-      <c r="A18" s="13">
+      <c r="A18" s="11">
         <v>17</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" s="14" t="s">
+      <c r="D18" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="14" t="s">
+      <c r="F18" s="12" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="19" ht="34" spans="1:6">
-      <c r="A19" s="13">
+      <c r="A19" s="11">
         <v>18</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E19" s="14" t="s">
+      <c r="D19" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="F19" s="14" t="s">
+      <c r="F19" s="12" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="20" ht="51" spans="1:6">
-      <c r="A20" s="13">
+      <c r="A20" s="11">
         <v>19</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="D20" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E20" s="14" t="s">
+      <c r="D20" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="F20" s="14" t="s">
+      <c r="F20" s="12" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="21" ht="34" spans="1:6">
-      <c r="A21" s="13">
+      <c r="A21" s="11">
         <v>20</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C21" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D21" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E21" s="14" t="s">
+      <c r="D21" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="F21" s="14" t="s">
+      <c r="F21" s="12" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="22" ht="34" spans="1:6">
-      <c r="A22" s="13">
+      <c r="A22" s="11">
         <v>21</v>
       </c>
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="C22" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D22" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E22" s="14" t="s">
+      <c r="D22" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="F22" s="14" t="s">
+      <c r="F22" s="12" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="23" ht="34" spans="1:6">
-      <c r="A23" s="13">
+      <c r="A23" s="11">
         <v>22</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D23" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E23" s="14" t="s">
+      <c r="D23" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="F23" s="14" t="s">
+      <c r="F23" s="12" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="24" ht="34" spans="1:6">
-      <c r="A24" s="13">
+      <c r="A24" s="11">
         <v>23</v>
       </c>
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="C24" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D24" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E24" s="14" t="s">
+      <c r="D24" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F24" s="14" t="s">
+      <c r="F24" s="12" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="25" ht="34" spans="1:6">
-      <c r="A25" s="13">
+      <c r="A25" s="11">
         <v>24</v>
       </c>
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C25" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="D25" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E25" s="14" t="s">
+      <c r="D25" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F25" s="14" t="s">
+      <c r="F25" s="12" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="26" ht="34" spans="1:6">
-      <c r="A26" s="13">
+      <c r="A26" s="11">
         <v>25</v>
       </c>
-      <c r="B26" s="14" t="s">
+      <c r="B26" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D26" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E26" s="14" t="s">
+      <c r="D26" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="F26" s="14" t="s">
+      <c r="F26" s="12" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="27" ht="51" spans="1:6">
-      <c r="A27" s="13">
+      <c r="A27" s="11">
         <v>26</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C27" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D27" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E27" s="14" t="s">
+      <c r="D27" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="14" t="s">
+      <c r="F27" s="12" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="28" ht="51" spans="1:6">
-      <c r="A28" s="13">
+      <c r="A28" s="11">
         <v>27</v>
       </c>
-      <c r="B28" s="14" t="s">
+      <c r="B28" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="C28" s="14" t="s">
+      <c r="C28" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="D28" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E28" s="14" t="s">
+      <c r="D28" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="F28" s="14" t="s">
+      <c r="F28" s="12" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="29" ht="51" spans="1:6">
-      <c r="A29" s="13">
+      <c r="A29" s="11">
         <v>28</v>
       </c>
-      <c r="B29" s="14" t="s">
+      <c r="B29" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="C29" s="14" t="s">
+      <c r="C29" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="D29" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E29" s="14" t="s">
+      <c r="D29" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="F29" s="14" t="s">
+      <c r="F29" s="12" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="30" ht="51" spans="1:6">
-      <c r="A30" s="13">
+      <c r="A30" s="11">
         <v>29</v>
       </c>
-      <c r="B30" s="14" t="s">
+      <c r="B30" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="C30" s="14" t="s">
+      <c r="C30" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="D30" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E30" s="14" t="s">
+      <c r="D30" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="F30" s="14" t="s">
+      <c r="F30" s="12" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="31" ht="51" spans="1:6">
-      <c r="A31" s="13">
+      <c r="A31" s="11">
         <v>30</v>
       </c>
-      <c r="B31" s="14" t="s">
+      <c r="B31" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C31" s="14" t="s">
+      <c r="C31" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="D31" s="14" t="s">
+      <c r="D31" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="E31" s="14" t="s">
+      <c r="E31" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="F31" s="14" t="s">
+      <c r="F31" s="12" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="32" ht="51" spans="1:6">
-      <c r="A32" s="13">
+      <c r="A32" s="11">
         <v>31</v>
       </c>
-      <c r="B32" s="14" t="s">
+      <c r="B32" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="C32" s="14" t="s">
+      <c r="C32" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="D32" s="14" t="s">
+      <c r="D32" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="E32" s="14" t="s">
+      <c r="E32" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="F32" s="14" t="s">
+      <c r="F32" s="12" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="33" ht="51" spans="1:6">
-      <c r="A33" s="13">
+      <c r="A33" s="11">
         <v>32</v>
       </c>
-      <c r="B33" s="14" t="s">
+      <c r="B33" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="C33" s="14" t="s">
+      <c r="C33" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="D33" s="14" t="s">
+      <c r="D33" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="E33" s="14" t="s">
+      <c r="E33" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="F33" s="14" t="s">
+      <c r="F33" s="12" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="34" ht="51" spans="1:6">
-      <c r="A34" s="13">
+      <c r="A34" s="11">
         <v>33</v>
       </c>
-      <c r="B34" s="14" t="s">
+      <c r="B34" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="C34" s="14" t="s">
+      <c r="C34" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="D34" s="14" t="s">
+      <c r="D34" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="E34" s="14" t="s">
+      <c r="E34" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="F34" s="14" t="s">
+      <c r="F34" s="12" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="35" ht="34" spans="1:6">
-      <c r="A35" s="13">
+      <c r="A35" s="11">
         <v>34</v>
       </c>
-      <c r="B35" s="14" t="s">
+      <c r="B35" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C35" s="14" t="s">
+      <c r="C35" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D35" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E35" s="14" t="s">
+      <c r="D35" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="F35" s="14" t="s">
+      <c r="F35" s="12" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="36" ht="51" spans="1:7">
-      <c r="A36" s="13">
+      <c r="A36" s="11">
         <v>35</v>
       </c>
-      <c r="B36" s="14" t="s">
+      <c r="B36" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="C36" s="14" t="s">
+      <c r="C36" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="D36" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E36" s="14" t="s">
+      <c r="D36" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E36" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="F36" s="14" t="s">
+      <c r="F36" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="G36" s="13" t="s">
+      <c r="G36" s="11" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="37" ht="101" spans="1:7">
-      <c r="A37" s="13">
+      <c r="A37" s="11">
         <v>36</v>
       </c>
-      <c r="B37" s="14" t="s">
+      <c r="B37" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="14" t="s">
+      <c r="C37" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="D37" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E37" s="14" t="s">
+      <c r="D37" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E37" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="F37" s="14" t="s">
+      <c r="F37" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="G37" s="13"/>
+      <c r="G37" s="11"/>
     </row>
     <row r="38" ht="101" spans="1:7">
-      <c r="A38" s="13">
+      <c r="A38" s="11">
         <v>37</v>
       </c>
-      <c r="B38" s="14" t="s">
+      <c r="B38" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="C38" s="14" t="s">
+      <c r="C38" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="D38" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E38" s="14" t="s">
+      <c r="D38" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E38" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="F38" s="14" t="s">
+      <c r="F38" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="G38" s="13"/>
+      <c r="G38" s="11"/>
     </row>
     <row r="39" ht="118" spans="1:7">
-      <c r="A39" s="13">
+      <c r="A39" s="11">
         <v>38</v>
       </c>
-      <c r="B39" s="14" t="s">
+      <c r="B39" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="C39" s="14" t="s">
+      <c r="C39" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="D39" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E39" s="14" t="s">
+      <c r="D39" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="F39" s="14" t="s">
+      <c r="F39" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="G39" s="13"/>
+      <c r="G39" s="11"/>
     </row>
     <row r="40" ht="51" spans="1:7">
-      <c r="A40" s="13">
+      <c r="A40" s="11">
         <v>39</v>
       </c>
-      <c r="B40" s="14" t="s">
+      <c r="B40" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="C40" s="14" t="s">
+      <c r="C40" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="D40" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E40" s="14" t="s">
+      <c r="D40" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E40" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="F40" s="14" t="s">
+      <c r="F40" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="G40" s="13"/>
+      <c r="G40" s="11"/>
     </row>
     <row r="41" ht="101" spans="1:7">
-      <c r="A41" s="13">
+      <c r="A41" s="11">
         <v>40</v>
       </c>
-      <c r="B41" s="14" t="s">
+      <c r="B41" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="C41" s="14" t="s">
+      <c r="C41" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="D41" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E41" s="14" t="s">
+      <c r="D41" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E41" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="F41" s="14" t="s">
+      <c r="F41" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="G41" s="14" t="s">
+      <c r="G41" s="12" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="42" ht="84" spans="1:7">
-      <c r="A42" s="13">
+      <c r="A42" s="11">
         <v>41</v>
       </c>
-      <c r="B42" s="14" t="s">
+      <c r="B42" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="C42" s="14" t="s">
+      <c r="C42" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="D42" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E42" s="14" t="s">
+      <c r="D42" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E42" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="F42" s="14" t="s">
+      <c r="F42" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="G42" s="14" t="s">
+      <c r="G42" s="12" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="43" ht="84" spans="1:7">
-      <c r="A43" s="13">
+      <c r="A43" s="11">
         <v>42</v>
       </c>
-      <c r="B43" s="14" t="s">
+      <c r="B43" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="C43" s="14" t="s">
+      <c r="C43" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="D43" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E43" s="14" t="s">
+      <c r="D43" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E43" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="F43" s="14" t="s">
+      <c r="F43" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="G43" s="14" t="s">
+      <c r="G43" s="12" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="44" ht="118" spans="1:7">
-      <c r="A44" s="13">
+      <c r="A44" s="11">
         <v>43</v>
       </c>
-      <c r="B44" s="14" t="s">
+      <c r="B44" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="C44" s="14" t="s">
+      <c r="C44" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="D44" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E44" s="14" t="s">
+      <c r="D44" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E44" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="F44" s="14" t="s">
+      <c r="F44" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="G44" s="14" t="s">
+      <c r="G44" s="12" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="45" ht="101" spans="1:7">
-      <c r="A45" s="13">
+      <c r="A45" s="11">
         <v>44</v>
       </c>
-      <c r="B45" s="14" t="s">
+      <c r="B45" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="C45" s="14" t="s">
+      <c r="C45" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="D45" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E45" s="14" t="s">
+      <c r="D45" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E45" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="F45" s="14" t="s">
+      <c r="F45" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="G45" s="14" t="s">
+      <c r="G45" s="12" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="46" ht="118" spans="1:7">
-      <c r="A46" s="13">
+      <c r="A46" s="11">
         <v>45</v>
       </c>
-      <c r="B46" s="14" t="s">
+      <c r="B46" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="C46" s="14" t="s">
+      <c r="C46" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="D46" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E46" s="14" t="s">
+      <c r="D46" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E46" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="F46" s="14" t="s">
+      <c r="F46" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="G46" s="14" t="s">
+      <c r="G46" s="12" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="47" ht="118" spans="1:7">
-      <c r="A47" s="13">
+      <c r="A47" s="11">
         <v>46</v>
       </c>
-      <c r="B47" s="14" t="s">
+      <c r="B47" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="C47" s="14" t="s">
+      <c r="C47" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="D47" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E47" s="14" t="s">
+      <c r="D47" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E47" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="F47" s="14" t="s">
+      <c r="F47" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="G47" s="14" t="s">
+      <c r="G47" s="12" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="48" ht="34" spans="1:7">
-      <c r="A48" s="13">
+      <c r="A48" s="11">
         <v>47</v>
       </c>
-      <c r="B48" s="14" t="s">
+      <c r="B48" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="C48" s="14" t="s">
+      <c r="C48" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="D48" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E48" s="14" t="s">
+      <c r="D48" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E48" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="F48" s="14" t="s">
+      <c r="F48" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="G48" s="14" t="s">
+      <c r="G48" s="12" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="49" ht="34" spans="1:7">
-      <c r="A49" s="13">
+      <c r="A49" s="11">
         <v>48</v>
       </c>
-      <c r="B49" s="14" t="s">
+      <c r="B49" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="C49" s="14" t="s">
+      <c r="C49" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="D49" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E49" s="14" t="s">
+      <c r="D49" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E49" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="F49" s="14" t="s">
+      <c r="F49" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="G49" s="14" t="s">
+      <c r="G49" s="12" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="50" ht="135" spans="1:7">
-      <c r="A50" s="13">
+      <c r="A50" s="11">
         <v>49</v>
       </c>
-      <c r="B50" s="14" t="s">
+      <c r="B50" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="C50" s="14" t="s">
+      <c r="C50" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="D50" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E50" s="14" t="s">
+      <c r="D50" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E50" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="F50" s="14" t="s">
+      <c r="F50" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="G50" s="14" t="s">
+      <c r="G50" s="12" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="51" ht="34" spans="1:7">
-      <c r="A51" s="13">
+      <c r="A51" s="11">
         <v>50</v>
       </c>
-      <c r="B51" s="14" t="s">
+      <c r="B51" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="C51" s="14" t="s">
+      <c r="C51" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="D51" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E51" s="14" t="s">
+      <c r="D51" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E51" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="F51" s="14" t="s">
+      <c r="F51" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="G51" s="14" t="s">
+      <c r="G51" s="12" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="52" ht="68" spans="1:7">
-      <c r="A52" s="13">
+      <c r="A52" s="11">
         <v>51</v>
       </c>
-      <c r="B52" s="14" t="s">
+      <c r="B52" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="C52" s="14" t="s">
+      <c r="C52" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="D52" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E52" s="14" t="s">
+      <c r="D52" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E52" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="F52" s="13" t="s">
+      <c r="F52" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="G52" s="13" t="s">
+      <c r="G52" s="11" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="53" ht="68" spans="1:7">
-      <c r="A53" s="13">
+      <c r="A53" s="11">
         <v>52</v>
       </c>
-      <c r="B53" s="14" t="s">
+      <c r="B53" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="C53" s="14" t="s">
+      <c r="C53" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="D53" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E53" s="14" t="s">
+      <c r="D53" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E53" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="F53" s="13"/>
-      <c r="G53" s="13"/>
+      <c r="F53" s="11"/>
+      <c r="G53" s="11"/>
     </row>
     <row r="54" ht="68" spans="1:7">
-      <c r="A54" s="13">
+      <c r="A54" s="11">
         <v>53</v>
       </c>
-      <c r="B54" s="14" t="s">
+      <c r="B54" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="C54" s="14" t="s">
+      <c r="C54" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="D54" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E54" s="14" t="s">
+      <c r="D54" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E54" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="F54" s="13"/>
-      <c r="G54" s="13"/>
+      <c r="F54" s="11"/>
+      <c r="G54" s="11"/>
     </row>
     <row r="55" ht="68" spans="1:7">
-      <c r="A55" s="13">
+      <c r="A55" s="11">
         <v>54</v>
       </c>
-      <c r="B55" s="14" t="s">
+      <c r="B55" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="C55" s="14" t="s">
+      <c r="C55" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="D55" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E55" s="14" t="s">
+      <c r="D55" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E55" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="F55" s="13"/>
-      <c r="G55" s="13"/>
+      <c r="F55" s="11"/>
+      <c r="G55" s="11"/>
     </row>
     <row r="56" ht="68" spans="1:7">
-      <c r="A56" s="13">
+      <c r="A56" s="11">
         <v>55</v>
       </c>
-      <c r="B56" s="14" t="s">
+      <c r="B56" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="C56" s="14" t="s">
+      <c r="C56" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="D56" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E56" s="14" t="s">
+      <c r="D56" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E56" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="F56" s="13"/>
-      <c r="G56" s="13"/>
+      <c r="F56" s="11"/>
+      <c r="G56" s="11"/>
     </row>
     <row r="57" ht="68" spans="1:7">
-      <c r="A57" s="13">
+      <c r="A57" s="11">
         <v>56</v>
       </c>
-      <c r="B57" s="14" t="s">
+      <c r="B57" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="C57" s="14" t="s">
+      <c r="C57" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="D57" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E57" s="14" t="s">
+      <c r="D57" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E57" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="F57" s="13"/>
-      <c r="G57" s="13"/>
+      <c r="F57" s="11"/>
+      <c r="G57" s="11"/>
     </row>
     <row r="58" ht="68" spans="1:7">
-      <c r="A58" s="13">
+      <c r="A58" s="11">
         <v>57</v>
       </c>
-      <c r="B58" s="14" t="s">
+      <c r="B58" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="C58" s="14" t="s">
+      <c r="C58" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="D58" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E58" s="14" t="s">
+      <c r="D58" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E58" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="F58" s="13"/>
-      <c r="G58" s="13"/>
+      <c r="F58" s="11"/>
+      <c r="G58" s="11"/>
     </row>
     <row r="59" ht="68" spans="1:7">
-      <c r="A59" s="13">
+      <c r="A59" s="11">
         <v>58</v>
       </c>
-      <c r="B59" s="14" t="s">
+      <c r="B59" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="C59" s="14" t="s">
+      <c r="C59" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="D59" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E59" s="14" t="s">
+      <c r="D59" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E59" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="F59" s="13"/>
-      <c r="G59" s="13"/>
+      <c r="F59" s="11"/>
+      <c r="G59" s="11"/>
     </row>
     <row r="60" ht="68" spans="1:7">
-      <c r="A60" s="13">
+      <c r="A60" s="11">
         <v>59</v>
       </c>
-      <c r="B60" s="14" t="s">
+      <c r="B60" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="C60" s="14" t="s">
+      <c r="C60" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="D60" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E60" s="14" t="s">
+      <c r="D60" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E60" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="F60" s="13"/>
-      <c r="G60" s="13"/>
+      <c r="F60" s="11"/>
+      <c r="G60" s="11"/>
     </row>
     <row r="61" ht="68" spans="1:7">
-      <c r="A61" s="13">
+      <c r="A61" s="11">
         <v>60</v>
       </c>
-      <c r="B61" s="14" t="s">
+      <c r="B61" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="C61" s="14" t="s">
+      <c r="C61" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="D61" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E61" s="14" t="s">
+      <c r="D61" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E61" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="F61" s="13"/>
-      <c r="G61" s="13"/>
+      <c r="F61" s="11"/>
+      <c r="G61" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -3735,59 +3726,59 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.8"/>
   <cols>
-    <col min="1" max="1" width="5.140625" style="13" customWidth="1"/>
-    <col min="2" max="2" width="34.140625" style="14" customWidth="1"/>
-    <col min="3" max="3" width="26.859375" style="14" customWidth="1"/>
-    <col min="4" max="4" width="24.859375" style="14" customWidth="1"/>
-    <col min="5" max="5" width="26.140625" style="14" customWidth="1"/>
-    <col min="6" max="6" width="26.2890625" style="14" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="15"/>
+    <col min="1" max="1" width="5.140625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="34.140625" style="12" customWidth="1"/>
+    <col min="3" max="3" width="26.859375" style="12" customWidth="1"/>
+    <col min="4" max="4" width="24.859375" style="12" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" style="12" customWidth="1"/>
+    <col min="6" max="6" width="26.2890625" style="12" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1" spans="1:6">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" s="12" customFormat="1" ht="20" customHeight="1" spans="1:6">
-      <c r="A2" s="17" t="s">
+    <row r="2" s="10" customFormat="1" ht="20" customHeight="1" spans="1:6">
+      <c r="A2" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="22"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="19"/>
     </row>
     <row r="3" ht="118" customHeight="1" spans="1:11">
-      <c r="A3" s="13">
+      <c r="A3" s="11">
         <v>1</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="E3" s="23" t="s">
+      <c r="E3" s="20" t="s">
         <v>112</v>
       </c>
       <c r="H3" s="1" t="s">
@@ -3798,1503 +3789,1503 @@
       <c r="K3" s="1"/>
     </row>
     <row r="4" ht="101" customHeight="1" spans="1:11">
-      <c r="A4" s="13">
+      <c r="A4" s="11">
         <v>2</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="E4" s="24"/>
+      <c r="E4" s="21"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" ht="122" customHeight="1" spans="1:11">
-      <c r="A5" s="13">
+      <c r="A5" s="11">
         <v>3</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="E5" s="24"/>
+      <c r="E5" s="21"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
     <row r="6" ht="84" spans="1:5">
-      <c r="A6" s="13">
+      <c r="A6" s="11">
         <v>4</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="E6" s="24"/>
+      <c r="E6" s="21"/>
     </row>
     <row r="7" customFormat="1" ht="84" spans="1:6">
-      <c r="A7" s="13">
+      <c r="A7" s="11">
         <v>5</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="E7" s="25"/>
-      <c r="F7" s="14"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="12"/>
     </row>
     <row r="8" customFormat="1" ht="84" spans="1:6">
-      <c r="A8" s="13">
+      <c r="A8" s="11">
         <v>6</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="E8" s="23" t="s">
+      <c r="E8" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="F8" s="14"/>
+      <c r="F8" s="12"/>
     </row>
     <row r="9" customFormat="1" ht="84" spans="1:6">
-      <c r="A9" s="13">
+      <c r="A9" s="11">
         <v>7</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="E9" s="24"/>
-      <c r="F9" s="14"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="12"/>
     </row>
     <row r="10" customFormat="1" ht="84" spans="1:6">
-      <c r="A10" s="13">
+      <c r="A10" s="11">
         <v>8</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="D10" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="E10" s="24"/>
-      <c r="F10" s="14"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="12"/>
     </row>
     <row r="11" customFormat="1" ht="84" spans="1:6">
-      <c r="A11" s="13">
-        <v>9</v>
-      </c>
-      <c r="B11" s="14" t="s">
+      <c r="A11" s="11">
+        <v>9</v>
+      </c>
+      <c r="B11" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="E11" s="24"/>
-      <c r="F11" s="14"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="12"/>
     </row>
     <row r="12" customFormat="1" ht="84" spans="1:6">
-      <c r="A12" s="13">
+      <c r="A12" s="11">
         <v>10</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="D12" s="19" t="s">
+      <c r="D12" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="E12" s="25"/>
-      <c r="F12" s="14"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="12"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="17" t="s">
         <v>120</v>
       </c>
-      <c r="B13" s="20"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
     </row>
     <row r="14" ht="84" spans="1:6">
-      <c r="A14" s="13">
+      <c r="A14" s="11">
         <v>11</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="E14" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="F14" s="14" t="s">
+      <c r="F14" s="12" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="15" ht="68" spans="1:6">
-      <c r="A15" s="13">
+      <c r="A15" s="11">
         <v>12</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="D15" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="E15" s="14" t="s">
+      <c r="E15" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="F15" s="14" t="s">
+      <c r="F15" s="12" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="16" ht="68" spans="1:6">
-      <c r="A16" s="13">
+      <c r="A16" s="11">
         <v>13</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="D16" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="E16" s="14" t="s">
+      <c r="E16" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="F16" s="14" t="s">
+      <c r="F16" s="12" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="17" ht="68" spans="1:6">
-      <c r="A17" s="13">
+      <c r="A17" s="11">
         <v>14</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="D17" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="E17" s="14" t="s">
+      <c r="E17" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="F17" s="14" t="s">
+      <c r="F17" s="12" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="18" ht="90" customHeight="1" spans="1:6">
-      <c r="A18" s="13">
+      <c r="A18" s="11">
         <v>15</v>
       </c>
-      <c r="B18" s="21" t="s">
+      <c r="B18" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="C18" s="21" t="s">
+      <c r="C18" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="D18" s="21" t="s">
+      <c r="D18" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="E18" s="21" t="s">
+      <c r="E18" s="18" t="s">
         <v>140</v>
       </c>
-      <c r="F18" s="21" t="s">
+      <c r="F18" s="18" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="19" ht="66" customHeight="1" spans="1:6">
-      <c r="A19" s="13">
+      <c r="A19" s="11">
         <v>16</v>
       </c>
-      <c r="B19" s="21" t="s">
+      <c r="B19" s="18" t="s">
         <v>142</v>
       </c>
-      <c r="C19" s="21" t="s">
+      <c r="C19" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="D19" s="21" t="s">
+      <c r="D19" s="18" t="s">
         <v>143</v>
       </c>
-      <c r="E19" s="21" t="s">
+      <c r="E19" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="F19" s="21" t="s">
+      <c r="F19" s="18" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="20" ht="79" customHeight="1" spans="1:6">
-      <c r="A20" s="13">
+      <c r="A20" s="11">
         <v>17</v>
       </c>
-      <c r="B20" s="21" t="s">
+      <c r="B20" s="18" t="s">
         <v>145</v>
       </c>
-      <c r="C20" s="21" t="s">
+      <c r="C20" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="D20" s="21" t="s">
+      <c r="D20" s="18" t="s">
         <v>146</v>
       </c>
-      <c r="E20" s="21" t="s">
+      <c r="E20" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="F20" s="21" t="s">
+      <c r="F20" s="18" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="21" ht="80" customHeight="1" spans="1:6">
-      <c r="A21" s="13">
+      <c r="A21" s="11">
         <v>18</v>
       </c>
-      <c r="B21" s="21" t="s">
+      <c r="B21" s="18" t="s">
         <v>149</v>
       </c>
-      <c r="C21" s="21" t="s">
+      <c r="C21" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="D21" s="21" t="s">
+      <c r="D21" s="18" t="s">
         <v>150</v>
       </c>
-      <c r="E21" s="21" t="s">
+      <c r="E21" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="F21" s="21" t="s">
+      <c r="F21" s="18" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="22" ht="17" customHeight="1" spans="1:6">
-      <c r="A22" s="20" t="s">
+      <c r="A22" s="17" t="s">
         <v>152</v>
       </c>
-      <c r="B22" s="20"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
     </row>
     <row r="23" ht="84" spans="1:6">
-      <c r="A23" s="13">
+      <c r="A23" s="11">
         <v>19</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="D23" s="14" t="s">
+      <c r="D23" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="E23" s="14" t="s">
+      <c r="E23" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="F23" s="14" t="s">
+      <c r="F23" s="12" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="24" ht="68" spans="1:6">
-      <c r="A24" s="13">
+      <c r="A24" s="11">
         <v>20</v>
       </c>
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="C24" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="D24" s="14" t="s">
+      <c r="D24" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="E24" s="14" t="s">
+      <c r="E24" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="F24" s="14" t="s">
+      <c r="F24" s="12" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="25" ht="68" spans="1:6">
-      <c r="A25" s="13">
+      <c r="A25" s="11">
         <v>21</v>
       </c>
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C25" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="D25" s="14" t="s">
+      <c r="D25" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="E25" s="14" t="s">
+      <c r="E25" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="F25" s="14" t="s">
+      <c r="F25" s="12" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="26" ht="68" spans="1:6">
-      <c r="A26" s="13">
+      <c r="A26" s="11">
         <v>22</v>
       </c>
-      <c r="B26" s="14" t="s">
+      <c r="B26" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="D26" s="14" t="s">
+      <c r="D26" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="E26" s="14" t="s">
+      <c r="E26" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="F26" s="14" t="s">
+      <c r="F26" s="12" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="27" ht="68" spans="1:6">
-      <c r="A27" s="13">
+      <c r="A27" s="11">
         <v>23</v>
       </c>
-      <c r="B27" s="21" t="s">
+      <c r="B27" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="C27" s="21" t="s">
+      <c r="C27" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="D27" s="21" t="s">
+      <c r="D27" s="18" t="s">
         <v>154</v>
       </c>
-      <c r="E27" s="21" t="s">
+      <c r="E27" s="18" t="s">
         <v>155</v>
       </c>
-      <c r="F27" s="21" t="s">
+      <c r="F27" s="18" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="28" ht="51" spans="1:6">
-      <c r="A28" s="13">
+      <c r="A28" s="11">
         <v>24</v>
       </c>
-      <c r="B28" s="21" t="s">
+      <c r="B28" s="18" t="s">
         <v>142</v>
       </c>
-      <c r="C28" s="21" t="s">
+      <c r="C28" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="D28" s="21" t="s">
+      <c r="D28" s="18" t="s">
         <v>143</v>
       </c>
-      <c r="E28" s="21" t="s">
+      <c r="E28" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="F28" s="21" t="s">
+      <c r="F28" s="18" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="29" ht="68" spans="1:6">
-      <c r="A29" s="13">
+      <c r="A29" s="11">
         <v>25</v>
       </c>
-      <c r="B29" s="21" t="s">
+      <c r="B29" s="18" t="s">
         <v>145</v>
       </c>
-      <c r="C29" s="21" t="s">
+      <c r="C29" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="D29" s="21" t="s">
+      <c r="D29" s="18" t="s">
         <v>146</v>
       </c>
-      <c r="E29" s="21" t="s">
+      <c r="E29" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="F29" s="21" t="s">
+      <c r="F29" s="18" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="30" ht="68" spans="1:6">
-      <c r="A30" s="13">
+      <c r="A30" s="11">
         <v>26</v>
       </c>
-      <c r="B30" s="21" t="s">
+      <c r="B30" s="18" t="s">
         <v>149</v>
       </c>
-      <c r="C30" s="21" t="s">
+      <c r="C30" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="D30" s="21" t="s">
+      <c r="D30" s="18" t="s">
         <v>150</v>
       </c>
-      <c r="E30" s="21" t="s">
+      <c r="E30" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="F30" s="21" t="s">
+      <c r="F30" s="18" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="20" t="s">
+      <c r="A31" s="17" t="s">
         <v>159</v>
       </c>
-      <c r="B31" s="20"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="17"/>
     </row>
     <row r="32" ht="68" spans="1:6">
-      <c r="A32" s="13">
+      <c r="A32" s="11">
         <v>27</v>
       </c>
-      <c r="B32" s="21" t="s">
+      <c r="B32" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="C32" s="21" t="s">
+      <c r="C32" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="D32" s="21" t="s">
+      <c r="D32" s="18" t="s">
         <v>154</v>
       </c>
-      <c r="E32" s="21" t="s">
+      <c r="E32" s="18" t="s">
         <v>160</v>
       </c>
-      <c r="F32" s="21" t="s">
+      <c r="F32" s="18" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="33" ht="51" spans="1:6">
-      <c r="A33" s="13">
+      <c r="A33" s="11">
         <v>28</v>
       </c>
-      <c r="B33" s="21" t="s">
+      <c r="B33" s="18" t="s">
         <v>142</v>
       </c>
-      <c r="C33" s="21" t="s">
+      <c r="C33" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="D33" s="21" t="s">
+      <c r="D33" s="18" t="s">
         <v>143</v>
       </c>
-      <c r="E33" s="21" t="s">
+      <c r="E33" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="F33" s="21" t="s">
+      <c r="F33" s="18" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="34" ht="68" spans="1:6">
-      <c r="A34" s="13">
+      <c r="A34" s="11">
         <v>29</v>
       </c>
-      <c r="B34" s="21" t="s">
+      <c r="B34" s="18" t="s">
         <v>145</v>
       </c>
-      <c r="C34" s="21" t="s">
+      <c r="C34" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="D34" s="21" t="s">
+      <c r="D34" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="E34" s="21" t="s">
+      <c r="E34" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="F34" s="21" t="s">
+      <c r="F34" s="18" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="35" ht="68" spans="1:6">
-      <c r="A35" s="13">
+      <c r="A35" s="11">
         <v>30</v>
       </c>
-      <c r="B35" s="21" t="s">
+      <c r="B35" s="18" t="s">
         <v>149</v>
       </c>
-      <c r="C35" s="21" t="s">
+      <c r="C35" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="D35" s="21" t="s">
+      <c r="D35" s="18" t="s">
         <v>162</v>
       </c>
-      <c r="E35" s="21" t="s">
+      <c r="E35" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="F35" s="21" t="s">
+      <c r="F35" s="18" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="36" spans="1:6">
-      <c r="A36" s="20" t="s">
+      <c r="A36" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="B36" s="20"/>
-      <c r="C36" s="20"/>
-      <c r="D36" s="20"/>
-      <c r="E36" s="20"/>
-      <c r="F36" s="20"/>
+      <c r="B36" s="17"/>
+      <c r="C36" s="17"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="17"/>
+      <c r="F36" s="17"/>
     </row>
     <row r="37" ht="84" spans="1:6">
-      <c r="A37" s="13">
+      <c r="A37" s="11">
         <v>31</v>
       </c>
-      <c r="B37" s="21" t="s">
+      <c r="B37" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="C37" s="21" t="s">
+      <c r="C37" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="D37" s="21" t="s">
+      <c r="D37" s="18" t="s">
         <v>164</v>
       </c>
-      <c r="E37" s="21" t="s">
+      <c r="E37" s="18" t="s">
         <v>165</v>
       </c>
-      <c r="F37" s="21" t="s">
+      <c r="F37" s="18" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="38" ht="68" spans="1:6">
-      <c r="A38" s="13">
+      <c r="A38" s="11">
         <v>32</v>
       </c>
-      <c r="B38" s="21" t="s">
+      <c r="B38" s="18" t="s">
         <v>142</v>
       </c>
-      <c r="C38" s="21" t="s">
+      <c r="C38" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="D38" s="21" t="s">
+      <c r="D38" s="18" t="s">
         <v>166</v>
       </c>
-      <c r="E38" s="21" t="s">
+      <c r="E38" s="18" t="s">
         <v>167</v>
       </c>
-      <c r="F38" s="21" t="s">
+      <c r="F38" s="18" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="39" ht="68" spans="1:6">
-      <c r="A39" s="13">
+      <c r="A39" s="11">
         <v>33</v>
       </c>
-      <c r="B39" s="21" t="s">
+      <c r="B39" s="18" t="s">
         <v>145</v>
       </c>
-      <c r="C39" s="21" t="s">
+      <c r="C39" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="D39" s="21" t="s">
+      <c r="D39" s="18" t="s">
         <v>168</v>
       </c>
-      <c r="E39" s="21" t="s">
+      <c r="E39" s="18" t="s">
         <v>169</v>
       </c>
-      <c r="F39" s="21" t="s">
+      <c r="F39" s="18" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="40" ht="68" spans="1:6">
-      <c r="A40" s="13">
+      <c r="A40" s="11">
         <v>34</v>
       </c>
-      <c r="B40" s="21" t="s">
+      <c r="B40" s="18" t="s">
         <v>149</v>
       </c>
-      <c r="C40" s="21" t="s">
+      <c r="C40" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="D40" s="21" t="s">
+      <c r="D40" s="18" t="s">
         <v>170</v>
       </c>
-      <c r="E40" s="21" t="s">
+      <c r="E40" s="18" t="s">
         <v>169</v>
       </c>
-      <c r="F40" s="21" t="s">
+      <c r="F40" s="18" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="41" spans="1:6">
-      <c r="A41" s="20" t="s">
+      <c r="A41" s="17" t="s">
         <v>171</v>
       </c>
-      <c r="B41" s="20"/>
-      <c r="C41" s="20"/>
-      <c r="D41" s="20"/>
-      <c r="E41" s="20"/>
-      <c r="F41" s="20"/>
+      <c r="B41" s="17"/>
+      <c r="C41" s="17"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="17"/>
+      <c r="F41" s="17"/>
     </row>
     <row r="42" ht="84" spans="1:6">
-      <c r="A42" s="13">
+      <c r="A42" s="11">
         <v>35</v>
       </c>
-      <c r="B42" s="14" t="s">
+      <c r="B42" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="C42" s="14" t="s">
+      <c r="C42" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="D42" s="21" t="s">
+      <c r="D42" s="18" t="s">
         <v>174</v>
       </c>
-      <c r="E42" s="14" t="s">
+      <c r="E42" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="F42" s="14" t="s">
+      <c r="F42" s="12" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="43" ht="68" spans="1:6">
-      <c r="A43" s="13">
+      <c r="A43" s="11">
         <v>36</v>
       </c>
-      <c r="B43" s="14" t="s">
+      <c r="B43" s="12" t="s">
         <v>176</v>
       </c>
-      <c r="C43" s="14" t="s">
+      <c r="C43" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="D43" s="21" t="s">
+      <c r="D43" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E43" s="14" t="s">
+      <c r="E43" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="F43" s="14" t="s">
+      <c r="F43" s="12" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="44" ht="68" spans="1:6">
-      <c r="A44" s="13">
+      <c r="A44" s="11">
         <v>37</v>
       </c>
-      <c r="B44" s="14" t="s">
+      <c r="B44" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="C44" s="14" t="s">
+      <c r="C44" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="D44" s="21" t="s">
+      <c r="D44" s="18" t="s">
         <v>180</v>
       </c>
-      <c r="E44" s="14" t="s">
+      <c r="E44" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="F44" s="14" t="s">
+      <c r="F44" s="12" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="45" ht="68" spans="1:6">
-      <c r="A45" s="13">
+      <c r="A45" s="11">
         <v>38</v>
       </c>
-      <c r="B45" s="14" t="s">
+      <c r="B45" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="C45" s="14" t="s">
+      <c r="C45" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="D45" s="21" t="s">
+      <c r="D45" s="18" t="s">
         <v>182</v>
       </c>
-      <c r="E45" s="14" t="s">
+      <c r="E45" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="F45" s="14" t="s">
+      <c r="F45" s="12" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="46" ht="68" spans="1:6">
-      <c r="A46" s="13">
+      <c r="A46" s="11">
         <v>39</v>
       </c>
-      <c r="B46" s="21" t="s">
+      <c r="B46" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="C46" s="21" t="s">
+      <c r="C46" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="D46" s="21" t="s">
+      <c r="D46" s="18" t="s">
         <v>184</v>
       </c>
-      <c r="E46" s="21" t="s">
+      <c r="E46" s="18" t="s">
         <v>160</v>
       </c>
-      <c r="F46" s="21" t="s">
+      <c r="F46" s="18" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="47" ht="118" spans="1:6">
-      <c r="A47" s="13">
+      <c r="A47" s="11">
         <v>40</v>
       </c>
-      <c r="B47" s="21" t="s">
+      <c r="B47" s="18" t="s">
         <v>142</v>
       </c>
-      <c r="C47" s="21" t="s">
+      <c r="C47" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="D47" s="21" t="s">
+      <c r="D47" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="E47" s="21" t="s">
+      <c r="E47" s="18" t="s">
         <v>187</v>
       </c>
-      <c r="F47" s="21" t="s">
+      <c r="F47" s="18" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="48" ht="68" spans="1:6">
-      <c r="A48" s="13">
+      <c r="A48" s="11">
         <v>41</v>
       </c>
-      <c r="B48" s="21" t="s">
+      <c r="B48" s="18" t="s">
         <v>145</v>
       </c>
-      <c r="C48" s="21" t="s">
+      <c r="C48" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="D48" s="21" t="s">
+      <c r="D48" s="18" t="s">
         <v>189</v>
       </c>
-      <c r="E48" s="21" t="s">
+      <c r="E48" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="F48" s="21" t="s">
+      <c r="F48" s="18" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="49" ht="68" spans="1:6">
-      <c r="A49" s="13">
+      <c r="A49" s="11">
         <v>42</v>
       </c>
-      <c r="B49" s="21" t="s">
+      <c r="B49" s="18" t="s">
         <v>149</v>
       </c>
-      <c r="C49" s="21" t="s">
+      <c r="C49" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="D49" s="21" t="s">
+      <c r="D49" s="18" t="s">
         <v>191</v>
       </c>
-      <c r="E49" s="21" t="s">
+      <c r="E49" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="F49" s="21" t="s">
+      <c r="F49" s="18" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="50" spans="1:6">
-      <c r="A50" s="20" t="s">
+      <c r="A50" s="17" t="s">
         <v>193</v>
       </c>
-      <c r="B50" s="20"/>
-      <c r="C50" s="20"/>
-      <c r="D50" s="20"/>
-      <c r="E50" s="20"/>
-      <c r="F50" s="20"/>
+      <c r="B50" s="17"/>
+      <c r="C50" s="17"/>
+      <c r="D50" s="17"/>
+      <c r="E50" s="17"/>
+      <c r="F50" s="17"/>
     </row>
     <row r="51" ht="68" spans="1:6">
-      <c r="A51" s="13">
+      <c r="A51" s="11">
         <v>43</v>
       </c>
-      <c r="B51" s="14" t="s">
+      <c r="B51" s="12" t="s">
         <v>194</v>
       </c>
-      <c r="C51" s="14" t="s">
+      <c r="C51" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="D51" s="14" t="s">
+      <c r="D51" s="12" t="s">
         <v>195</v>
       </c>
-      <c r="E51" s="14" t="s">
+      <c r="E51" s="12" t="s">
         <v>196</v>
       </c>
-      <c r="F51" s="14" t="s">
+      <c r="F51" s="12" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="52" ht="68" spans="1:6">
-      <c r="A52" s="13">
+      <c r="A52" s="11">
         <v>44</v>
       </c>
-      <c r="B52" s="14" t="s">
+      <c r="B52" s="12" t="s">
         <v>198</v>
       </c>
-      <c r="C52" s="14" t="s">
+      <c r="C52" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="D52" s="14" t="s">
+      <c r="D52" s="12" t="s">
         <v>199</v>
       </c>
-      <c r="E52" s="14" t="s">
+      <c r="E52" s="12" t="s">
         <v>196</v>
       </c>
-      <c r="F52" s="14" t="s">
+      <c r="F52" s="12" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="53" ht="68" spans="1:6">
-      <c r="A53" s="13">
+      <c r="A53" s="11">
         <v>45</v>
       </c>
-      <c r="B53" s="14" t="s">
+      <c r="B53" s="12" t="s">
         <v>201</v>
       </c>
-      <c r="C53" s="14" t="s">
+      <c r="C53" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="D53" s="14" t="s">
+      <c r="D53" s="12" t="s">
         <v>202</v>
       </c>
-      <c r="E53" s="14" t="s">
+      <c r="E53" s="12" t="s">
         <v>196</v>
       </c>
-      <c r="F53" s="14" t="s">
+      <c r="F53" s="12" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="54" ht="68" spans="1:6">
-      <c r="A54" s="13">
+      <c r="A54" s="11">
         <v>46</v>
       </c>
-      <c r="B54" s="14" t="s">
+      <c r="B54" s="12" t="s">
         <v>204</v>
       </c>
-      <c r="C54" s="21" t="s">
+      <c r="C54" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="D54" s="21" t="s">
+      <c r="D54" s="18" t="s">
         <v>205</v>
       </c>
-      <c r="E54" s="21" t="s">
+      <c r="E54" s="18" t="s">
         <v>160</v>
       </c>
-      <c r="F54" s="21" t="s">
+      <c r="F54" s="18" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="55" ht="68" spans="1:6">
-      <c r="A55" s="13">
+      <c r="A55" s="11">
         <v>47</v>
       </c>
-      <c r="B55" s="14" t="s">
+      <c r="B55" s="12" t="s">
         <v>206</v>
       </c>
-      <c r="C55" s="21" t="s">
+      <c r="C55" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="D55" s="21" t="s">
+      <c r="D55" s="18" t="s">
         <v>207</v>
       </c>
-      <c r="E55" s="21" t="s">
+      <c r="E55" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="F55" s="21" t="s">
+      <c r="F55" s="18" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="56" ht="68" spans="1:6">
-      <c r="A56" s="13">
+      <c r="A56" s="11">
         <v>48</v>
       </c>
-      <c r="B56" s="14" t="s">
+      <c r="B56" s="12" t="s">
         <v>208</v>
       </c>
-      <c r="C56" s="21" t="s">
+      <c r="C56" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="D56" s="21" t="s">
+      <c r="D56" s="18" t="s">
         <v>209</v>
       </c>
-      <c r="E56" s="21" t="s">
+      <c r="E56" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="F56" s="21" t="s">
+      <c r="F56" s="18" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="57" ht="68" spans="1:6">
-      <c r="A57" s="13">
+      <c r="A57" s="11">
         <v>49</v>
       </c>
-      <c r="B57" s="14" t="s">
+      <c r="B57" s="12" t="s">
         <v>210</v>
       </c>
-      <c r="C57" s="21" t="s">
+      <c r="C57" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="D57" s="21" t="s">
+      <c r="D57" s="18" t="s">
         <v>211</v>
       </c>
-      <c r="E57" s="21" t="s">
+      <c r="E57" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="F57" s="21" t="s">
+      <c r="F57" s="18" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="58" spans="1:6">
-      <c r="A58" s="20" t="s">
+      <c r="A58" s="17" t="s">
         <v>212</v>
       </c>
-      <c r="B58" s="20"/>
-      <c r="C58" s="20"/>
-      <c r="D58" s="20"/>
-      <c r="E58" s="20"/>
-      <c r="F58" s="20"/>
+      <c r="B58" s="17"/>
+      <c r="C58" s="17"/>
+      <c r="D58" s="17"/>
+      <c r="E58" s="17"/>
+      <c r="F58" s="17"/>
     </row>
     <row r="59" ht="84" spans="1:6">
-      <c r="A59" s="13">
+      <c r="A59" s="11">
         <v>50</v>
       </c>
-      <c r="B59" s="14" t="s">
+      <c r="B59" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="C59" s="14" t="s">
+      <c r="C59" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="D59" s="21" t="s">
+      <c r="D59" s="18" t="s">
         <v>213</v>
       </c>
-      <c r="E59" s="14" t="s">
+      <c r="E59" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="F59" s="14" t="s">
+      <c r="F59" s="12" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="60" ht="68" spans="1:6">
-      <c r="A60" s="13">
+      <c r="A60" s="11">
         <v>51</v>
       </c>
-      <c r="B60" s="14" t="s">
+      <c r="B60" s="12" t="s">
         <v>176</v>
       </c>
-      <c r="C60" s="14" t="s">
+      <c r="C60" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="D60" s="21" t="s">
+      <c r="D60" s="18" t="s">
         <v>214</v>
       </c>
-      <c r="E60" s="14" t="s">
+      <c r="E60" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="F60" s="14" t="s">
+      <c r="F60" s="12" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="61" ht="68" spans="1:6">
-      <c r="A61" s="13">
+      <c r="A61" s="11">
         <v>52</v>
       </c>
-      <c r="B61" s="14" t="s">
+      <c r="B61" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="C61" s="14" t="s">
+      <c r="C61" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="D61" s="21" t="s">
+      <c r="D61" s="18" t="s">
         <v>215</v>
       </c>
-      <c r="E61" s="14" t="s">
+      <c r="E61" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="F61" s="14" t="s">
+      <c r="F61" s="12" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="62" ht="68" spans="1:6">
-      <c r="A62" s="13">
+      <c r="A62" s="11">
         <v>53</v>
       </c>
-      <c r="B62" s="14" t="s">
+      <c r="B62" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="C62" s="14" t="s">
+      <c r="C62" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="D62" s="21" t="s">
+      <c r="D62" s="18" t="s">
         <v>216</v>
       </c>
-      <c r="E62" s="14" t="s">
+      <c r="E62" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="F62" s="14" t="s">
+      <c r="F62" s="12" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="63" ht="68" spans="1:6">
-      <c r="A63" s="13">
+      <c r="A63" s="11">
         <v>54</v>
       </c>
-      <c r="B63" s="21" t="s">
+      <c r="B63" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="C63" s="21" t="s">
+      <c r="C63" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="D63" s="21" t="s">
+      <c r="D63" s="18" t="s">
         <v>217</v>
       </c>
-      <c r="E63" s="21" t="s">
+      <c r="E63" s="18" t="s">
         <v>218</v>
       </c>
-      <c r="F63" s="21" t="s">
+      <c r="F63" s="18" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="64" ht="84" spans="1:6">
-      <c r="A64" s="13">
+      <c r="A64" s="11">
         <v>55</v>
       </c>
-      <c r="B64" s="21" t="s">
+      <c r="B64" s="18" t="s">
         <v>142</v>
       </c>
-      <c r="C64" s="21" t="s">
+      <c r="C64" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="D64" s="21" t="s">
+      <c r="D64" s="18" t="s">
         <v>214</v>
       </c>
-      <c r="E64" s="21" t="s">
+      <c r="E64" s="18" t="s">
         <v>220</v>
       </c>
-      <c r="F64" s="21" t="s">
+      <c r="F64" s="18" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="65" ht="84" spans="1:6">
-      <c r="A65" s="13">
+      <c r="A65" s="11">
         <v>56</v>
       </c>
-      <c r="B65" s="21" t="s">
+      <c r="B65" s="18" t="s">
         <v>145</v>
       </c>
-      <c r="C65" s="21" t="s">
+      <c r="C65" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="D65" s="21" t="s">
+      <c r="D65" s="18" t="s">
         <v>221</v>
       </c>
-      <c r="E65" s="21" t="s">
+      <c r="E65" s="18" t="s">
         <v>220</v>
       </c>
-      <c r="F65" s="21" t="s">
+      <c r="F65" s="18" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="66" ht="68" spans="1:6">
-      <c r="A66" s="13">
+      <c r="A66" s="11">
         <v>57</v>
       </c>
-      <c r="B66" s="21" t="s">
+      <c r="B66" s="18" t="s">
         <v>149</v>
       </c>
-      <c r="C66" s="21" t="s">
+      <c r="C66" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="D66" s="21" t="s">
+      <c r="D66" s="18" t="s">
         <v>222</v>
       </c>
-      <c r="E66" s="21" t="s">
+      <c r="E66" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="F66" s="21" t="s">
+      <c r="F66" s="18" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="67" spans="1:6">
-      <c r="A67" s="20" t="s">
+      <c r="A67" s="17" t="s">
         <v>223</v>
       </c>
-      <c r="B67" s="20"/>
-      <c r="C67" s="20"/>
-      <c r="D67" s="20"/>
-      <c r="E67" s="20"/>
-      <c r="F67" s="20"/>
+      <c r="B67" s="17"/>
+      <c r="C67" s="17"/>
+      <c r="D67" s="17"/>
+      <c r="E67" s="17"/>
+      <c r="F67" s="17"/>
     </row>
     <row r="68" ht="84" spans="1:6">
-      <c r="A68" s="13">
+      <c r="A68" s="11">
         <v>58</v>
       </c>
-      <c r="B68" s="14" t="s">
+      <c r="B68" s="12" t="s">
         <v>224</v>
       </c>
-      <c r="C68" s="14" t="s">
+      <c r="C68" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="D68" s="21" t="s">
+      <c r="D68" s="18" t="s">
         <v>225</v>
       </c>
-      <c r="E68" s="14" t="s">
+      <c r="E68" s="12" t="s">
         <v>226</v>
       </c>
-      <c r="F68" s="14" t="s">
+      <c r="F68" s="12" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="69" ht="68" spans="1:6">
-      <c r="A69" s="13">
+      <c r="A69" s="11">
         <v>59</v>
       </c>
-      <c r="B69" s="14" t="s">
+      <c r="B69" s="12" t="s">
         <v>228</v>
       </c>
-      <c r="C69" s="14" t="s">
+      <c r="C69" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="D69" s="21" t="s">
+      <c r="D69" s="18" t="s">
         <v>229</v>
       </c>
-      <c r="E69" s="14" t="s">
+      <c r="E69" s="12" t="s">
         <v>230</v>
       </c>
-      <c r="F69" s="14" t="s">
+      <c r="F69" s="12" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="70" ht="68" spans="1:6">
-      <c r="A70" s="13">
+      <c r="A70" s="11">
         <v>60</v>
       </c>
-      <c r="B70" s="14" t="s">
+      <c r="B70" s="12" t="s">
         <v>232</v>
       </c>
-      <c r="C70" s="14" t="s">
+      <c r="C70" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="D70" s="21" t="s">
+      <c r="D70" s="18" t="s">
         <v>233</v>
       </c>
-      <c r="E70" s="14" t="s">
+      <c r="E70" s="12" t="s">
         <v>234</v>
       </c>
-      <c r="F70" s="14" t="s">
+      <c r="F70" s="12" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="71" ht="68" spans="1:6">
-      <c r="A71" s="13">
+      <c r="A71" s="11">
         <v>61</v>
       </c>
-      <c r="B71" s="14" t="s">
+      <c r="B71" s="12" t="s">
         <v>236</v>
       </c>
-      <c r="C71" s="14" t="s">
+      <c r="C71" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="D71" s="21" t="s">
+      <c r="D71" s="18" t="s">
         <v>237</v>
       </c>
-      <c r="E71" s="14" t="s">
+      <c r="E71" s="12" t="s">
         <v>234</v>
       </c>
-      <c r="F71" s="14" t="s">
+      <c r="F71" s="12" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="72" ht="68" spans="1:6">
-      <c r="A72" s="13">
+      <c r="A72" s="11">
         <v>62</v>
       </c>
-      <c r="B72" s="21" t="s">
+      <c r="B72" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="C72" s="21" t="s">
+      <c r="C72" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="D72" s="21" t="s">
+      <c r="D72" s="18" t="s">
         <v>239</v>
       </c>
-      <c r="E72" s="21" t="s">
+      <c r="E72" s="18" t="s">
         <v>240</v>
       </c>
-      <c r="F72" s="21" t="s">
+      <c r="F72" s="18" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="73" ht="68" spans="1:6">
-      <c r="A73" s="13">
+      <c r="A73" s="11">
         <v>63</v>
       </c>
-      <c r="B73" s="21" t="s">
+      <c r="B73" s="18" t="s">
         <v>142</v>
       </c>
-      <c r="C73" s="21" t="s">
+      <c r="C73" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="D73" s="21" t="s">
+      <c r="D73" s="18" t="s">
         <v>229</v>
       </c>
-      <c r="E73" s="21" t="s">
+      <c r="E73" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="F73" s="21" t="s">
+      <c r="F73" s="18" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="74" ht="68" spans="1:6">
-      <c r="A74" s="13">
+      <c r="A74" s="11">
         <v>64</v>
       </c>
-      <c r="B74" s="21" t="s">
+      <c r="B74" s="18" t="s">
         <v>242</v>
       </c>
-      <c r="C74" s="21" t="s">
+      <c r="C74" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="D74" s="21" t="s">
+      <c r="D74" s="18" t="s">
         <v>243</v>
       </c>
-      <c r="E74" s="21" t="s">
+      <c r="E74" s="18" t="s">
         <v>244</v>
       </c>
-      <c r="F74" s="21" t="s">
+      <c r="F74" s="18" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="75" ht="68" spans="1:6">
-      <c r="A75" s="13">
+      <c r="A75" s="11">
         <v>65</v>
       </c>
-      <c r="B75" s="21" t="s">
+      <c r="B75" s="18" t="s">
         <v>245</v>
       </c>
-      <c r="C75" s="21" t="s">
+      <c r="C75" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="D75" s="21" t="s">
+      <c r="D75" s="18" t="s">
         <v>246</v>
       </c>
-      <c r="E75" s="21" t="s">
+      <c r="E75" s="18" t="s">
         <v>244</v>
       </c>
-      <c r="F75" s="21" t="s">
+      <c r="F75" s="18" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="76" spans="1:6">
-      <c r="A76" s="20" t="s">
+      <c r="A76" s="17" t="s">
         <v>247</v>
       </c>
-      <c r="B76" s="20"/>
-      <c r="C76" s="20"/>
-      <c r="D76" s="20"/>
-      <c r="E76" s="20"/>
-      <c r="F76" s="20"/>
+      <c r="B76" s="17"/>
+      <c r="C76" s="17"/>
+      <c r="D76" s="17"/>
+      <c r="E76" s="17"/>
+      <c r="F76" s="17"/>
     </row>
     <row r="77" ht="84" spans="1:6">
-      <c r="A77" s="13">
+      <c r="A77" s="11">
         <v>66</v>
       </c>
-      <c r="B77" s="14" t="s">
+      <c r="B77" s="12" t="s">
         <v>224</v>
       </c>
-      <c r="C77" s="14" t="s">
+      <c r="C77" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="D77" s="21" t="s">
+      <c r="D77" s="18" t="s">
         <v>248</v>
       </c>
-      <c r="E77" s="14" t="s">
+      <c r="E77" s="12" t="s">
         <v>226</v>
       </c>
-      <c r="F77" s="14" t="s">
+      <c r="F77" s="12" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="78" ht="68" spans="1:6">
-      <c r="A78" s="13">
+      <c r="A78" s="11">
         <v>67</v>
       </c>
-      <c r="B78" s="14" t="s">
+      <c r="B78" s="12" t="s">
         <v>249</v>
       </c>
-      <c r="C78" s="14" t="s">
+      <c r="C78" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="D78" s="21" t="s">
+      <c r="D78" s="18" t="s">
         <v>229</v>
       </c>
-      <c r="E78" s="14" t="s">
+      <c r="E78" s="12" t="s">
         <v>230</v>
       </c>
-      <c r="F78" s="14" t="s">
+      <c r="F78" s="12" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="79" ht="68" spans="1:6">
-      <c r="A79" s="13">
+      <c r="A79" s="11">
         <v>68</v>
       </c>
-      <c r="B79" s="14" t="s">
+      <c r="B79" s="12" t="s">
         <v>232</v>
       </c>
-      <c r="C79" s="14" t="s">
+      <c r="C79" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="D79" s="21" t="s">
+      <c r="D79" s="18" t="s">
         <v>233</v>
       </c>
-      <c r="E79" s="14" t="s">
+      <c r="E79" s="12" t="s">
         <v>234</v>
       </c>
-      <c r="F79" s="14" t="s">
+      <c r="F79" s="12" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="80" ht="68" spans="1:6">
-      <c r="A80" s="13">
+      <c r="A80" s="11">
         <v>69</v>
       </c>
-      <c r="B80" s="14" t="s">
+      <c r="B80" s="12" t="s">
         <v>236</v>
       </c>
-      <c r="C80" s="14" t="s">
+      <c r="C80" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="D80" s="21" t="s">
+      <c r="D80" s="18" t="s">
         <v>237</v>
       </c>
-      <c r="E80" s="14" t="s">
+      <c r="E80" s="12" t="s">
         <v>250</v>
       </c>
-      <c r="F80" s="14" t="s">
+      <c r="F80" s="12" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="81" ht="68" spans="1:6">
-      <c r="A81" s="13">
+      <c r="A81" s="11">
         <v>70</v>
       </c>
-      <c r="B81" s="21" t="s">
+      <c r="B81" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="C81" s="21" t="s">
+      <c r="C81" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="D81" s="21" t="s">
+      <c r="D81" s="18" t="s">
         <v>239</v>
       </c>
-      <c r="E81" s="21" t="s">
+      <c r="E81" s="18" t="s">
         <v>160</v>
       </c>
-      <c r="F81" s="21" t="s">
+      <c r="F81" s="18" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="82" ht="68" spans="1:6">
-      <c r="A82" s="13">
+      <c r="A82" s="11">
         <v>71</v>
       </c>
-      <c r="B82" s="21" t="s">
+      <c r="B82" s="18" t="s">
         <v>142</v>
       </c>
-      <c r="C82" s="21" t="s">
+      <c r="C82" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="D82" s="21" t="s">
+      <c r="D82" s="18" t="s">
         <v>229</v>
       </c>
-      <c r="E82" s="21" t="s">
+      <c r="E82" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="F82" s="21" t="s">
+      <c r="F82" s="18" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="83" ht="68" spans="1:6">
-      <c r="A83" s="13">
+      <c r="A83" s="11">
         <v>72</v>
       </c>
-      <c r="B83" s="21" t="s">
+      <c r="B83" s="18" t="s">
         <v>242</v>
       </c>
-      <c r="C83" s="21" t="s">
+      <c r="C83" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="D83" s="21" t="s">
+      <c r="D83" s="18" t="s">
         <v>243</v>
       </c>
-      <c r="E83" s="21" t="s">
+      <c r="E83" s="18" t="s">
         <v>244</v>
       </c>
-      <c r="F83" s="21" t="s">
+      <c r="F83" s="18" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="84" ht="68" spans="1:6">
-      <c r="A84" s="13">
+      <c r="A84" s="11">
         <v>73</v>
       </c>
-      <c r="B84" s="21" t="s">
+      <c r="B84" s="18" t="s">
         <v>245</v>
       </c>
-      <c r="C84" s="21" t="s">
+      <c r="C84" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="D84" s="21" t="s">
+      <c r="D84" s="18" t="s">
         <v>246</v>
       </c>
-      <c r="E84" s="21" t="s">
+      <c r="E84" s="18" t="s">
         <v>244</v>
       </c>
-      <c r="F84" s="21" t="s">
+      <c r="F84" s="18" t="s">
         <v>192</v>
       </c>
     </row>
@@ -5325,551 +5316,537 @@
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D38" sqref="D38"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="4.296875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="26.953125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="23.1796875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="18.359375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="25.6484375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="18.875" style="4" customWidth="1"/>
-    <col min="7" max="16384" width="9" style="5"/>
+    <col min="1" max="1" width="4.296875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.953125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="23.1796875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="18.359375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="25.6484375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="18.875" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="20" customHeight="1" spans="1:6">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" s="2" customFormat="1" ht="20" customHeight="1" spans="1:6">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="11"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="9"/>
     </row>
     <row r="3" ht="34" spans="1:5">
-      <c r="A3" s="3">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="4" ht="84" spans="1:5">
-      <c r="A4" s="3">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="5" s="3" customFormat="1" spans="1:1">
-      <c r="A5" s="3" t="s">
+    <row r="5" s="1" customFormat="1" spans="1:1">
+      <c r="A5" s="1" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="6" ht="34" spans="1:6">
-      <c r="A6" s="3">
+      <c r="A6" s="1">
         <v>3</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="3" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="7" ht="51" spans="1:6">
-      <c r="A7" s="3">
+    <row r="7" ht="51" spans="1:5">
+      <c r="A7" s="1">
         <v>4</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="F7" s="9"/>
-    </row>
-    <row r="8" ht="51" spans="1:6">
-      <c r="A8" s="3">
+    </row>
+    <row r="8" ht="34" spans="1:5">
+      <c r="A8" s="1">
         <v>5</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="F8" s="9"/>
-    </row>
-    <row r="9" s="3" customFormat="1" spans="1:1">
-      <c r="A9" s="3">
-        <v>6</v>
+    </row>
+    <row r="9" s="1" customFormat="1" spans="1:1">
+      <c r="A9" s="1" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="10" ht="68" spans="1:5">
-      <c r="A10" s="3">
+      <c r="A10" s="1">
         <v>7</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>266</v>
-      </c>
-      <c r="C10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>268</v>
       </c>
+      <c r="E10" s="3" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="11" ht="68" spans="1:6">
-      <c r="A11" s="3">
+      <c r="A11" s="1">
         <v>8</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>269</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="C11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>271</v>
       </c>
+      <c r="F11" s="3" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="12" ht="68" spans="1:5">
-      <c r="A12" s="3">
-        <v>9</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>272</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="13" s="3" customFormat="1" spans="1:1">
-      <c r="A13" s="3" t="s">
+      <c r="A12" s="1">
+        <v>9</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>273</v>
       </c>
+      <c r="C12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="13" s="1" customFormat="1" spans="1:1">
+      <c r="A13" s="1" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="14" ht="84" spans="1:5">
-      <c r="A14" s="3">
+      <c r="A14" s="1">
         <v>10</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>274</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="15" ht="34" spans="1:6">
-      <c r="A15" s="3">
+      <c r="C14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="15" ht="34" spans="1:5">
+      <c r="A15" s="1">
         <v>11</v>
       </c>
-      <c r="B15" s="9" t="s">
-        <v>276</v>
-      </c>
-      <c r="C15" s="9" t="s">
+      <c r="B15" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9" t="s">
+      <c r="C15" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="F15" s="9"/>
-    </row>
-    <row r="16" ht="84" spans="1:6">
-      <c r="A16" s="3">
+      <c r="E15" s="3" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="16" ht="84" spans="1:5">
+      <c r="A16" s="1">
         <v>12</v>
       </c>
-      <c r="B16" s="9" t="s">
-        <v>279</v>
-      </c>
-      <c r="C16" s="9" t="s">
+      <c r="B16" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9" t="s">
+      <c r="C16" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="F16" s="9"/>
-    </row>
-    <row r="17" ht="84" spans="1:6">
-      <c r="A17" s="3">
+      <c r="E16" s="3" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="17" ht="84" spans="1:5">
+      <c r="A17" s="1">
         <v>13</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="18" ht="84" spans="1:5">
+      <c r="A18" s="1">
+        <v>14</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="20" ht="85" customHeight="1" spans="1:5">
+      <c r="A20" s="1">
+        <v>15</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="21" ht="51" spans="1:5">
+      <c r="A21" s="1">
+        <v>16</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="22" ht="51" spans="1:5">
+      <c r="A22" s="1">
+        <v>17</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="23" ht="51" spans="1:5">
+      <c r="A23" s="1">
+        <v>18</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="E23" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="C17" s="9" t="s">
-        <v>283</v>
-      </c>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9" t="s">
-        <v>284</v>
-      </c>
-      <c r="F17" s="9"/>
-    </row>
-    <row r="18" ht="84" spans="1:6">
-      <c r="A18" s="3">
-        <v>14</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>285</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>286</v>
-      </c>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9" t="s">
-        <v>287</v>
-      </c>
-      <c r="F18" s="9"/>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-    </row>
-    <row r="20" ht="85" customHeight="1" spans="1:5">
-      <c r="A20" s="3">
-        <v>15</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>289</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>290</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="21" ht="51" spans="1:5">
-      <c r="A21" s="3">
-        <v>16</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>292</v>
-      </c>
-      <c r="C21" s="4" t="s">
+    </row>
+    <row r="24" ht="51" spans="1:5">
+      <c r="A24" s="1">
+        <v>19</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="25" ht="68" spans="1:5">
+      <c r="A25" s="1">
+        <v>20</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="26" ht="84" spans="1:6">
+      <c r="A26" s="1">
+        <v>21</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="E21" s="4" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="22" ht="51" spans="1:5">
-      <c r="A22" s="3">
-        <v>17</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>295</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>293</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="23" ht="51" spans="1:5">
-      <c r="A23" s="3">
-        <v>18</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>297</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>298</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="24" ht="51" spans="1:5">
-      <c r="A24" s="3">
-        <v>19</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>297</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>299</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="25" ht="68" spans="1:5">
-      <c r="A25" s="3">
-        <v>20</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>297</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>301</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="26" ht="84" spans="1:6">
-      <c r="A26" s="3">
-        <v>21</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>292</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>303</v>
-      </c>
-      <c r="E26" s="4" t="s">
+      <c r="C26" s="3" t="s">
         <v>304</v>
       </c>
-      <c r="F26" s="4" t="s">
+      <c r="E26" s="3" t="s">
         <v>305</v>
       </c>
+      <c r="F26" s="3" t="s">
+        <v>306</v>
+      </c>
     </row>
     <row r="27" ht="84" spans="1:5">
-      <c r="A27" s="3">
+      <c r="A27" s="1">
         <v>22</v>
       </c>
-      <c r="B27" s="4" t="s">
-        <v>306</v>
-      </c>
-      <c r="C27" s="4" t="s">
+      <c r="B27" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="C27" s="3" t="s">
         <v>308</v>
       </c>
+      <c r="E27" s="3" t="s">
+        <v>309</v>
+      </c>
     </row>
     <row r="28" ht="51" spans="1:5">
-      <c r="A28" s="3">
+      <c r="A28" s="1">
         <v>23</v>
       </c>
-      <c r="B28" s="4" t="s">
-        <v>306</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>309</v>
-      </c>
-      <c r="E28" s="4" t="s">
+      <c r="B28" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>310</v>
       </c>
+      <c r="E28" s="3" t="s">
+        <v>311</v>
+      </c>
     </row>
     <row r="29" ht="34" spans="1:5">
-      <c r="A29" s="3">
+      <c r="A29" s="1">
         <v>24</v>
       </c>
-      <c r="B29" s="4" t="s">
-        <v>311</v>
-      </c>
-      <c r="C29" s="4" t="s">
+      <c r="B29" s="3" t="s">
         <v>312</v>
       </c>
-      <c r="E29" s="4" t="s">
-        <v>281</v>
+      <c r="C29" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="30" ht="84" spans="1:5">
-      <c r="A30" s="3">
+      <c r="A30" s="1">
         <v>25</v>
       </c>
-      <c r="B30" s="4" t="s">
-        <v>311</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>313</v>
-      </c>
-      <c r="E30" s="4" t="s">
+      <c r="B30" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="C30" s="8" t="s">
         <v>314</v>
       </c>
+      <c r="E30" s="3" t="s">
+        <v>315</v>
+      </c>
     </row>
     <row r="31" ht="51" spans="1:5">
-      <c r="A31" s="3">
+      <c r="A31" s="1">
         <v>26</v>
       </c>
-      <c r="B31" s="4" t="s">
-        <v>311</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>315</v>
-      </c>
-      <c r="E31" s="4" t="s">
+      <c r="B31" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>316</v>
       </c>
+      <c r="E31" s="3" t="s">
+        <v>317</v>
+      </c>
     </row>
     <row r="32" ht="51" spans="1:5">
-      <c r="A32" s="3">
+      <c r="A32" s="1">
         <v>27</v>
       </c>
-      <c r="B32" s="4" t="s">
-        <v>311</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>317</v>
-      </c>
-      <c r="E32" s="4" t="s">
+      <c r="B32" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="C32" s="3" t="s">
         <v>318</v>
       </c>
+      <c r="E32" s="3" t="s">
+        <v>319</v>
+      </c>
     </row>
     <row r="33" ht="34" spans="1:5">
-      <c r="A33" s="3">
+      <c r="A33" s="1">
         <v>28</v>
       </c>
-      <c r="B33" s="4" t="s">
-        <v>311</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>319</v>
-      </c>
-      <c r="E33" s="4" t="s">
+      <c r="B33" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="C33" s="3" t="s">
         <v>320</v>
       </c>
+      <c r="E33" s="3" t="s">
+        <v>321</v>
+      </c>
     </row>
     <row r="34" ht="51" spans="1:5">
-      <c r="A34" s="3">
+      <c r="A34" s="1">
         <v>29</v>
       </c>
-      <c r="B34" s="4" t="s">
-        <v>311</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>321</v>
-      </c>
-      <c r="E34" s="4" t="s">
+      <c r="B34" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>322</v>
       </c>
+      <c r="E34" s="3" t="s">
+        <v>323</v>
+      </c>
     </row>
     <row r="35" ht="17" spans="1:5">
-      <c r="A35" s="3">
+      <c r="A35" s="1">
         <v>30</v>
       </c>
-      <c r="B35" s="4" t="s">
-        <v>306</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>323</v>
-      </c>
-      <c r="E35" s="4" t="s">
+      <c r="B35" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="C35" s="3" t="s">
         <v>324</v>
       </c>
+      <c r="E35" s="3" t="s">
+        <v>325</v>
+      </c>
     </row>
     <row r="36" ht="84" spans="1:5">
-      <c r="A36" s="3">
+      <c r="A36" s="1">
         <v>31</v>
       </c>
-      <c r="B36" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="C36" s="4" t="s">
+      <c r="B36" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C36" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="E36" s="4" t="s">
-        <v>326</v>
+      <c r="E36" s="3" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="37" ht="68" spans="1:6">
-      <c r="A37" s="3">
+      <c r="A37" s="1">
         <v>32</v>
       </c>
-      <c r="B37" s="4" t="s">
-        <v>306</v>
-      </c>
-      <c r="C37" s="4" t="s">
+      <c r="B37" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="38" ht="84" spans="1:5">
+      <c r="A38" s="1">
+        <v>33</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E38" s="3" t="s">
         <v>327</v>
       </c>
-      <c r="E37" s="4" t="s">
-        <v>328</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="38" ht="84" spans="1:5">
-      <c r="A38" s="3">
-        <v>33</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>326</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A5:F5"/>
+    <mergeCell ref="A9:F9"/>
     <mergeCell ref="A13:F13"/>
     <mergeCell ref="A19:F19"/>
     <mergeCell ref="F6:F8"/>

</xml_diff>

<commit_message>
multy Eviroment IOS test
</commit_message>
<xml_diff>
--- a/Log/Magic_eraser_test_log.xlsx
+++ b/Log/Magic_eraser_test_log.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19020" windowHeight="14880" firstSheet="2" activeTab="2"/>
+    <workbookView windowWidth="18960" windowHeight="14940" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Image_selector_test" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="338">
   <si>
     <t>TC</t>
   </si>
@@ -802,6 +802,9 @@
     <t>Nhấn vào phần "image carousel"</t>
   </si>
   <si>
+    <t>chọn banner "Remove background" ở mục "Basic Tool"</t>
+  </si>
+  <si>
     <t>Bảng chọn ảnh ("Image Selector")</t>
   </si>
   <si>
@@ -871,7 +874,7 @@
     <t>Hiển thị dialog cảnh bảo đang thoát ra mà chưa lưu kết quả</t>
   </si>
   <si>
-    <t>Ở màn "Home-edit", trên màn đang có dialog cảnh báo thoát ra mà chưa lưu kết quả, màn hình bị 1 lớp layer xám phủ lên, các nút trên màn bị vô hiệu hoá</t>
+    <t>Ở màn "Home-edit", Màn hình hiển thị trạng thái mờ (overlay) bởi lớp phủ xám, toàn bộ nút chức năng bị disable.</t>
   </si>
   <si>
     <t>Chọn vùng bên ngoài 2 nút trên dialog</t>
@@ -880,18 +883,12 @@
     <t>App không có phản hồi</t>
   </si>
   <si>
-    <t>Ở màn "Home-edit", trên màn đang có dialog cảnh báo thoát ra mà chưa lưu kết quả, màn hình bị 2 lớp layer xám phủ lên, các nút trên màn bị vô hiệu hoá</t>
-  </si>
-  <si>
     <t>Chọn button tiếp tục chỉnh sửa</t>
   </si>
   <si>
     <t>Ở lại màn "Home-edit", dialog cảnh báo biến mất</t>
   </si>
   <si>
-    <t>Ở màn "Home-edit", trên màn đang có dialog cảnh báo thoát ra mà chưa lưu kết quả, màn hình bị 3 lớp layer xám phủ lên, các nút trên màn bị vô hiệu hoá</t>
-  </si>
-  <si>
     <t>chọn button xác nhận thoát ra</t>
   </si>
   <si>
@@ -1025,6 +1022,34 @@
   </si>
   <si>
     <t>Ở màn "Home edit", trên màn đang có bảng chọn ảnh</t>
+  </si>
+  <si>
+    <t>Test GUI tính tương thích cho từng thiết bị và cỡ màn hình (trọng tâm vào GUI)</t>
+  </si>
+  <si>
+    <t>Ở màn "Home", Thiết bị: iPhoneX [IOS 15.0]</t>
+  </si>
+  <si>
+    <t>1. Chọn button "Remove BG"
+2. Chọn ảnh
+3. Chọn cutout-edit
+4. Chọn Save 
+5. Chọn 1 Template bất kỳ
+6. Chọn Save ở màn hình Edit Basic 
+7. Chọn Back ở màn hình Home edit 
+8. chọn button đồng ý thoát ra ở dialog cảnh báo</t>
+  </si>
+  <si>
+    <t>Màn hình chuyển mượt mà theo thứ tự Home, Home-edit, Edit-cutout, Home-edit, Edit-Basic, Home-edit, Home</t>
+  </si>
+  <si>
+    <t>Ở màn "Home", Thiết bị: iPhoneXs [IOS 18.5]</t>
+  </si>
+  <si>
+    <t>Ở màn "Home", Thiết bị: iPhone17 [IOS 26.0]</t>
+  </si>
+  <si>
+    <t>Ở màn "Home", Thiết bị: iPad  Pro 11-inch [IOS 26.0]</t>
   </si>
 </sst>
 </file>
@@ -5313,12 +5338,12 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
+      <selection pane="bottomLeft" activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="5"/>
@@ -5390,466 +5415,534 @@
         <v>254</v>
       </c>
     </row>
-    <row r="5" s="1" customFormat="1" spans="1:1">
-      <c r="A5" s="1" t="s">
+    <row r="5" s="3" customFormat="1" ht="51" spans="1:5">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="6" ht="34" spans="1:6">
-      <c r="A6" s="1">
+      <c r="E5" s="3" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="6" s="1" customFormat="1" spans="1:1">
+      <c r="A6" s="1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="7" ht="34" spans="1:6">
+      <c r="A7" s="1">
         <v>3</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="C6" s="3" t="s">
+      <c r="B7" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="F6" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="7" ht="51" spans="1:5">
-      <c r="A7" s="1">
+      <c r="F7" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="8" ht="51" spans="1:5">
+      <c r="A8" s="1">
         <v>4</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>261</v>
-      </c>
-      <c r="C7" s="3" t="s">
+      <c r="B8" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="C8" s="3" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="8" ht="34" spans="1:5">
-      <c r="A8" s="1">
+      <c r="E8" s="3" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="9" ht="34" spans="1:5">
+      <c r="A9" s="1">
         <v>5</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>264</v>
-      </c>
-      <c r="C8" s="3" t="s">
+      <c r="B9" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="9" s="1" customFormat="1" spans="1:1">
-      <c r="A9" s="1" t="s">
+      <c r="C9" s="3" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="10" ht="68" spans="1:5">
-      <c r="A10" s="1">
+      <c r="E9" s="3" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="10" s="1" customFormat="1" spans="1:1">
+      <c r="A10" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="11" ht="68" spans="1:5">
+      <c r="A11" s="1">
         <v>6</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="C10" s="3" t="s">
+      <c r="B11" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="11" ht="68" spans="1:6">
-      <c r="A11" s="1">
+      <c r="E11" s="3" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="12" ht="68" spans="1:6">
+      <c r="A12" s="1">
         <v>7</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>270</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="3" t="s">
+      <c r="B12" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="C12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="12" ht="68" spans="1:5">
-      <c r="A12" s="1">
+      <c r="F12" s="3" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="13" ht="68" spans="1:5">
+      <c r="A13" s="1">
         <v>8</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>273</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="13" s="1" customFormat="1" spans="1:1">
-      <c r="A13" s="1" t="s">
+      <c r="B13" s="3" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="14" ht="84" spans="1:5">
-      <c r="A14" s="1">
-        <v>9</v>
-      </c>
-      <c r="B14" s="3" t="s">
+      <c r="C13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="14" s="1" customFormat="1" spans="1:1">
+      <c r="A14" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="3" t="s">
+    </row>
+    <row r="15" ht="84" spans="1:5">
+      <c r="A15" s="1">
+        <v>9</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="15" ht="34" spans="1:5">
-      <c r="A15" s="1">
+      <c r="C15" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="16" ht="34" spans="1:5">
+      <c r="A16" s="1">
         <v>10</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>277</v>
-      </c>
-      <c r="C15" s="3" t="s">
+      <c r="B16" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="C16" s="3" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="16" ht="84" spans="1:5">
-      <c r="A16" s="1">
+      <c r="E16" s="3" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="17" ht="68" spans="1:5">
+      <c r="A17" s="1">
         <v>11</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="C16" s="3" t="s">
+      <c r="B17" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="C17" s="3" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="17" ht="84" spans="1:5">
-      <c r="A17" s="1">
+      <c r="E17" s="3" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="18" ht="68" spans="1:5">
+      <c r="A18" s="1">
         <v>12</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="C17" s="3" t="s">
+      <c r="B18" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E18" s="3" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="18" ht="84" spans="1:5">
-      <c r="A18" s="1">
+    <row r="19" ht="68" spans="1:5">
+      <c r="A19" s="1">
         <v>13</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B19" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="E19" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="E18" s="3" t="s">
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="1" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
-      <c r="A19" s="1" t="s">
+    <row r="21" ht="85" customHeight="1" spans="1:5">
+      <c r="A21" s="1">
+        <v>14</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="20" ht="85" customHeight="1" spans="1:5">
-      <c r="A20" s="1">
-        <v>14</v>
-      </c>
-      <c r="B20" s="3" t="s">
+      <c r="C21" s="3" t="s">
         <v>290</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="E21" s="3" t="s">
         <v>291</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="21" ht="51" spans="1:5">
-      <c r="A21" s="1">
-        <v>15</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>293</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>294</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="22" ht="51" spans="1:5">
       <c r="A22" s="1">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="C22" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="E22" s="3" t="s">
         <v>294</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="23" ht="51" spans="1:5">
       <c r="A23" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>282</v>
+        <v>296</v>
       </c>
     </row>
     <row r="24" ht="51" spans="1:5">
       <c r="A24" s="1">
+        <v>17</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="25" ht="51" spans="1:5">
+      <c r="A25" s="1">
         <v>18</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>298</v>
-      </c>
-      <c r="C24" s="3" t="s">
+      <c r="B25" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="E25" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="E24" s="3" t="s">
+    </row>
+    <row r="26" ht="68" spans="1:5">
+      <c r="A26" s="1">
+        <v>19</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="25" ht="68" spans="1:5">
-      <c r="A25" s="1">
-        <v>19</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>298</v>
-      </c>
-      <c r="C25" s="3" t="s">
+      <c r="E26" s="3" t="s">
         <v>302</v>
       </c>
-      <c r="E25" s="3" t="s">
+    </row>
+    <row r="27" ht="84" spans="1:6">
+      <c r="A27" s="1">
+        <v>20</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="26" ht="84" spans="1:6">
-      <c r="A26" s="1">
-        <v>20</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>293</v>
-      </c>
-      <c r="C26" s="3" t="s">
+      <c r="E27" s="3" t="s">
         <v>304</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="F27" s="3" t="s">
         <v>305</v>
       </c>
-      <c r="F26" s="3" t="s">
+    </row>
+    <row r="28" ht="84" spans="1:5">
+      <c r="A28" s="1">
+        <v>21</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="27" ht="84" spans="1:5">
-      <c r="A27" s="1">
-        <v>21</v>
-      </c>
-      <c r="B27" s="3" t="s">
+      <c r="C28" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="E28" s="3" t="s">
         <v>308</v>
       </c>
-      <c r="E27" s="3" t="s">
+    </row>
+    <row r="29" ht="51" spans="1:5">
+      <c r="A29" s="1">
+        <v>22</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="28" ht="51" spans="1:5">
-      <c r="A28" s="1">
-        <v>22</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>307</v>
-      </c>
-      <c r="C28" s="3" t="s">
+      <c r="E29" s="3" t="s">
         <v>310</v>
       </c>
-      <c r="E28" s="3" t="s">
+    </row>
+    <row r="30" ht="34" spans="1:5">
+      <c r="A30" s="1">
+        <v>23</v>
+      </c>
+      <c r="B30" s="3" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="29" ht="34" spans="1:5">
-      <c r="A29" s="1">
-        <v>23</v>
-      </c>
-      <c r="B29" s="3" t="s">
+      <c r="C30" s="3" t="s">
         <v>312</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="E30" s="3" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="31" ht="84" spans="1:5">
+      <c r="A31" s="1">
+        <v>24</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="C31" s="8" t="s">
         <v>313</v>
       </c>
-      <c r="E29" s="3" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="30" ht="84" spans="1:5">
-      <c r="A30" s="1">
-        <v>24</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>312</v>
-      </c>
-      <c r="C30" s="8" t="s">
+      <c r="E31" s="3" t="s">
         <v>314</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="31" ht="51" spans="1:5">
-      <c r="A31" s="1">
-        <v>25</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>312</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>316</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="32" ht="51" spans="1:5">
       <c r="A32" s="1">
+        <v>25</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="33" ht="51" spans="1:5">
+      <c r="A33" s="1">
         <v>26</v>
       </c>
-      <c r="B32" s="3" t="s">
-        <v>312</v>
-      </c>
-      <c r="C32" s="3" t="s">
+      <c r="B33" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="E33" s="3" t="s">
         <v>318</v>
       </c>
-      <c r="E32" s="3" t="s">
+    </row>
+    <row r="34" ht="34" spans="1:5">
+      <c r="A34" s="1">
+        <v>27</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="33" ht="34" spans="1:5">
-      <c r="A33" s="1">
-        <v>27</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>312</v>
-      </c>
-      <c r="C33" s="3" t="s">
+      <c r="E34" s="3" t="s">
         <v>320</v>
       </c>
-      <c r="E33" s="3" t="s">
+    </row>
+    <row r="35" ht="51" spans="1:5">
+      <c r="A35" s="1">
+        <v>28</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="C35" s="3" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="34" ht="51" spans="1:5">
-      <c r="A34" s="1">
-        <v>28</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>312</v>
-      </c>
-      <c r="C34" s="3" t="s">
+      <c r="E35" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="E34" s="3" t="s">
+    </row>
+    <row r="36" ht="17" spans="1:5">
+      <c r="A36" s="1">
+        <v>29</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="C36" s="3" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="35" ht="17" spans="1:5">
-      <c r="A35" s="1">
-        <v>29</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>307</v>
-      </c>
-      <c r="C35" s="3" t="s">
+      <c r="E36" s="3" t="s">
         <v>324</v>
       </c>
-      <c r="E35" s="3" t="s">
+    </row>
+    <row r="37" ht="84" spans="1:5">
+      <c r="A37" s="1">
+        <v>30</v>
+      </c>
+      <c r="B37" s="3" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="36" ht="84" spans="1:5">
-      <c r="A36" s="1">
-        <v>30</v>
-      </c>
-      <c r="B36" s="3" t="s">
+      <c r="C37" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E37" s="3" t="s">
         <v>326</v>
       </c>
-      <c r="C36" s="3" t="s">
+    </row>
+    <row r="38" ht="68" spans="1:6">
+      <c r="A38" s="1">
+        <v>31</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="39" ht="84" spans="1:5">
+      <c r="A39" s="1">
+        <v>32</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="C39" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="E36" s="3" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="37" ht="68" spans="1:6">
-      <c r="A37" s="1">
-        <v>31</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>307</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>328</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>329</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="38" ht="84" spans="1:5">
-      <c r="A38" s="1">
-        <v>32</v>
-      </c>
-      <c r="B38" s="3" t="s">
+      <c r="E39" s="3" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="C38" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>327</v>
-      </c>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+    </row>
+    <row r="41" ht="67" customHeight="1" spans="1:5">
+      <c r="A41" s="1">
+        <v>33</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="42" ht="67" customHeight="1" spans="2:5">
+      <c r="B42" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="C42" s="1"/>
+      <c r="E42" s="1"/>
+    </row>
+    <row r="43" ht="67" customHeight="1" spans="1:5">
+      <c r="A43" s="1">
+        <v>34</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="C43" s="1"/>
+      <c r="E43" s="1"/>
+    </row>
+    <row r="44" ht="76" customHeight="1" spans="1:5">
+      <c r="A44" s="1">
+        <v>35</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="C44" s="1"/>
+      <c r="E44" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="9">
     <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A5:F5"/>
-    <mergeCell ref="A9:F9"/>
-    <mergeCell ref="A13:F13"/>
-    <mergeCell ref="A19:F19"/>
-    <mergeCell ref="F6:F8"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A14:F14"/>
+    <mergeCell ref="A20:F20"/>
+    <mergeCell ref="A40:F40"/>
+    <mergeCell ref="C41:C44"/>
+    <mergeCell ref="E41:E44"/>
+    <mergeCell ref="F7:F9"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>